<commit_message>
Mini correction pour regarder lighthouse
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fred/Desktop/OpenClassRoom/P4 Vrac/ProjetP4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C4041AA-3381-A041-977E-E7CA3605A0AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08C01EF7-4481-2A43-BAFE-E3D391C612BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3100" yWindow="4780" windowWidth="46880" windowHeight="19880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -469,13 +469,13 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>3803650</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>25400</xdr:rowOff>
+      <xdr:colOff>6915150</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4464050" cy="749300"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="ZoneTexte 1">
@@ -489,7 +489,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="7499350" y="6121400"/>
+              <a:off x="10610850" y="6083300"/>
               <a:ext cx="4464050" cy="749300"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -811,7 +811,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback xmlns="">
+      <mc:Fallback>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="ZoneTexte 1">
@@ -825,7 +825,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="7499350" y="6121400"/>
+              <a:off x="10610850" y="6083300"/>
               <a:ext cx="4464050" cy="749300"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -853,11 +853,12 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="fr-FR" sz="1100" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
                 </a:rPr>
-                <a:t>𝑓(𝑥)=𝑎_0+∑24_(𝑛=1)^∞▒(𝑎_𝑛  cos⁡〖𝑛</a:t>
+                <a:t>𝑓(𝑥)=𝑎_0+∑_(𝑛=1)^∞▒(𝑎_𝑛  cos⁡〖𝑛</a:t>
               </a:r>
               <a:r>
                 <a:rPr lang="el-GR" sz="1100" i="0">
@@ -1111,7 +1112,7 @@
   <dimension ref="A1:Z1011"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
GRos changements pour accessbilité je galere
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fred/Desktop/OpenClassRoom/P4 Vrac/ProjetP4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16A0643-6CA3-1547-8E29-08A5B1E28E59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{728EB47D-C5F7-7D40-AB12-632EF45C9197}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3100" yWindow="4780" windowWidth="46880" windowHeight="19880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="93">
   <si>
     <t>Catégorie</t>
   </si>
@@ -304,6 +304,12 @@
   </si>
   <si>
     <t>col-sm4 encadré plus visible</t>
+  </si>
+  <si>
+    <t>alt contenait paris</t>
+  </si>
+  <si>
+    <t>liens partenraire blackhat</t>
   </si>
 </sst>
 </file>
@@ -1115,7 +1121,7 @@
   <dimension ref="A1:Z1011"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1671,9 +1677,17 @@
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="34" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C34" t="s">
+        <v>91</v>
+      </c>
+    </row>
     <row r="35" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C36" t="s">
+        <v>92</v>
+      </c>
+    </row>
     <row r="37" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="38" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="39" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Video OpenClass Room accessibilité
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fred/Desktop/OpenClassRoom/P4 Vrac/ProjetP4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BC62CD0-6858-0448-8947-8372D38DB753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B4B099D-7DFE-6844-842D-1EDCF74E199E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3100" yWindow="4780" windowWidth="46880" windowHeight="19880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="95">
   <si>
     <t>Catégorie</t>
   </si>
@@ -310,6 +310,12 @@
   </si>
   <si>
     <t>liens partenraire blackhat</t>
+  </si>
+  <si>
+    <t>installer l'extension chrome wave</t>
+  </si>
+  <si>
+    <t>Lien Wave</t>
   </si>
 </sst>
 </file>
@@ -408,7 +414,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -426,6 +432,7 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -479,12 +486,12 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>4603750</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>38</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4464050" cy="749300"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="ZoneTexte 1">
@@ -820,7 +827,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="ZoneTexte 1">
@@ -905,8 +912,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E796EE32-1DFE-CD45-A2AF-F728FFC58B5F}" name="Tableau1" displayName="Tableau1" ref="A1:G30" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:G30" xr:uid="{E796EE32-1DFE-CD45-A2AF-F728FFC58B5F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E796EE32-1DFE-CD45-A2AF-F728FFC58B5F}" name="Tableau1" displayName="Tableau1" ref="A1:G38" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:G38" xr:uid="{E796EE32-1DFE-CD45-A2AF-F728FFC58B5F}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{9BB85078-D1DA-EA4F-939E-EA2B94AC6A91}" name="Catégorie"/>
     <tableColumn id="2" xr3:uid="{701895DD-CBC8-C945-8BB8-1AF30E309D3E}" name="Problème identifié"/>
@@ -1118,10 +1125,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1011"/>
+  <dimension ref="A1:Z1018"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1460,27 +1467,6 @@
       </c>
       <c r="G15" s="8"/>
     </row>
-    <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B16" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>74</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E16" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F16" t="s">
-        <v>12</v>
-      </c>
-      <c r="G16" s="8"/>
-    </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5" t="s">
         <v>7</v>
@@ -1614,92 +1600,170 @@
       <c r="G23" s="8"/>
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="5"/>
+      <c r="B24" t="s">
+        <v>92</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
       <c r="E24" s="4"/>
+      <c r="F24" s="5"/>
       <c r="G24" s="8"/>
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="A25" s="5"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="8"/>
+    </row>
+    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="5"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="8"/>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E27" s="4"/>
+      <c r="G27" s="8"/>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>41</v>
       </c>
-      <c r="B25" t="s">
+      <c r="B28" t="s">
         <v>42</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C28" t="s">
         <v>43</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D28" t="s">
         <v>44</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="E28" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="F28" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="G25" s="8"/>
-    </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="G28" s="8"/>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>41</v>
       </c>
-      <c r="B26" s="5" t="s">
+      <c r="B29" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="C29" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D29" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="E26" s="4" t="s">
+      <c r="E29" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="F29" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="G26" s="8"/>
-    </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="5" t="s">
+      <c r="G29" s="8"/>
+    </row>
+    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>41</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C30" s="5" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="33" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C33" t="s">
+    <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F31" t="s">
+        <v>12</v>
+      </c>
+      <c r="G31" s="8"/>
+    </row>
+    <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34" t="s">
+        <v>13</v>
+      </c>
       <c r="C34" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="35" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C36" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="37" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="39" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="40" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="41" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="46" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="47" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="48" spans="3:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+        <v>14</v>
+      </c>
+      <c r="D34" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F34" t="s">
+        <v>12</v>
+      </c>
+      <c r="G34" s="8"/>
+    </row>
+    <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C38" t="s">
+        <v>93</v>
+      </c>
+      <c r="D38" s="11" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="46" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="47" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="49" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="50" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="51" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2663,16 +2727,24 @@
     <row r="1009" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1010" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1011" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1012" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1013" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1014" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1015" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1016" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1017" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1018" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C11" r:id="rId1" display="https://fredericguilet.github.io/P4Guillet_Frederic25072021/voiture.com" xr:uid="{F0E0A3CD-37FD-9E44-B979-49DC1760F2BE}"/>
     <hyperlink ref="C12" r:id="rId2" display="https://fredericguilet.github.io/P4Guillet_Frederic25072021/pizza.com" xr:uid="{68CF73CC-7EFC-0048-B22E-4CE39E7A4D9F}"/>
+    <hyperlink ref="D38" r:id="rId3" xr:uid="{8B9623D5-26B1-F54A-9395-E5EC71494DBA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId3"/>
+  <drawing r:id="rId4"/>
   <tableParts count="1">
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ajout du mailto pour accessbilité?
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fred/Desktop/OpenClassRoom/P4 Vrac/ProjetP4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B4B099D-7DFE-6844-842D-1EDCF74E199E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C00701-F6DD-A24B-B6DC-4A4855B508E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3100" yWindow="4780" windowWidth="46880" windowHeight="19880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="98">
   <si>
     <t>Catégorie</t>
   </si>
@@ -108,9 +108,6 @@
     <t>Keyword</t>
   </si>
   <si>
-    <t>aujourdhui cela peut etre considérer comme une tentative de mauvais referement et se faire allumer</t>
-  </si>
-  <si>
     <t>la virer</t>
   </si>
   <si>
@@ -228,9 +225,6 @@
     <t>moi-même</t>
   </si>
   <si>
-    <t>Agence web à paris, stratégie web, web design, illustrations, design de site web, site web, web, internet, site internet, site</t>
-  </si>
-  <si>
     <t>Partenaires</t>
   </si>
   <si>
@@ -316,6 +310,21 @@
   </si>
   <si>
     <t>Lien Wave</t>
+  </si>
+  <si>
+    <t>Agence web à paris, stratégie web, web design, illustrations, des…..</t>
+  </si>
+  <si>
+    <t>BlackHat  considérer comme une tentative de mauvais referement et se faire allumer</t>
+  </si>
+  <si>
+    <t>Je l'ai viré on est a Lyon</t>
+  </si>
+  <si>
+    <t>changé en ombre plus propre</t>
+  </si>
+  <si>
+    <t>Je les ai viré aucun rapport et blackHat</t>
   </si>
 </sst>
 </file>
@@ -1128,17 +1137,17 @@
   <dimension ref="A1:Z1018"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="78.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="66.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="33.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="70.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="48.7109375" customWidth="1"/>
+    <col min="6" max="6" width="26" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.28515625" style="9" bestFit="1" customWidth="1"/>
     <col min="8" max="27" width="10.5703125" customWidth="1"/>
   </cols>
@@ -1163,7 +1172,7 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -1212,7 +1221,7 @@
         <v>12</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1256,7 +1265,7 @@
         <v>12</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1288,13 +1297,13 @@
         <v>24</v>
       </c>
       <c r="C7" t="s">
+        <v>94</v>
+      </c>
+      <c r="D7" t="s">
         <v>25</v>
       </c>
-      <c r="D7" t="s">
-        <v>26</v>
-      </c>
       <c r="E7" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F7" t="s">
         <v>12</v>
@@ -1303,19 +1312,19 @@
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
         <v>27</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="D8" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>30</v>
       </c>
       <c r="F8" t="s">
         <v>12</v>
@@ -1324,22 +1333,22 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
         <v>31</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="D9" t="s">
         <v>32</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="D9" t="s">
-        <v>33</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>23</v>
       </c>
       <c r="F9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G9" s="8"/>
     </row>
@@ -1348,19 +1357,19 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D10" t="s">
         <v>35</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="D10" t="s">
-        <v>36</v>
       </c>
       <c r="E10" s="4" t="s">
         <v>23</v>
       </c>
       <c r="F10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G10" s="8"/>
     </row>
@@ -1369,13 +1378,13 @@
         <v>7</v>
       </c>
       <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="D11" t="s">
         <v>37</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D11" t="s">
-        <v>38</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>23</v>
@@ -1390,13 +1399,13 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
+        <v>38</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" t="s">
         <v>39</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="D12" t="s">
-        <v>40</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>23</v>
@@ -1411,17 +1420,17 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D13" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E13" s="4"/>
       <c r="F13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G13" s="8"/>
     </row>
@@ -1430,19 +1439,19 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="F14" s="5" t="s">
         <v>46</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>47</v>
       </c>
       <c r="G14" s="8"/>
     </row>
@@ -1451,19 +1460,19 @@
         <v>7</v>
       </c>
       <c r="B15" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>51</v>
-      </c>
       <c r="F15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G15" s="8"/>
     </row>
@@ -1472,16 +1481,16 @@
         <v>7</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>54</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>55</v>
       </c>
       <c r="D17" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G17" s="8"/>
     </row>
@@ -1490,17 +1499,17 @@
         <v>7</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C18" s="6" t="s">
-        <v>58</v>
-      </c>
       <c r="D18" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E18" s="4"/>
       <c r="F18" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G18" s="8"/>
     </row>
@@ -1509,19 +1518,19 @@
         <v>7</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>61</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>62</v>
       </c>
       <c r="D19" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E19" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="F19" s="5" t="s">
         <v>63</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>64</v>
       </c>
       <c r="G19" s="8"/>
     </row>
@@ -1530,19 +1539,19 @@
         <v>7</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D20" s="5" t="s">
         <v>10</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G20" s="8"/>
     </row>
@@ -1551,15 +1560,15 @@
         <v>7</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="4"/>
       <c r="F21" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G21" s="8"/>
     </row>
@@ -1568,19 +1577,19 @@
         <v>7</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D22" s="5" t="s">
         <v>23</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F22" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G22" s="8"/>
     </row>
@@ -1589,10 +1598,10 @@
         <v>7</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D23" s="5"/>
       <c r="E23" s="4"/>
@@ -1602,9 +1611,11 @@
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="5"/>
       <c r="B24" t="s">
-        <v>92</v>
-      </c>
-      <c r="C24" s="5"/>
+        <v>90</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>97</v>
+      </c>
       <c r="D24" s="5"/>
       <c r="E24" s="4"/>
       <c r="F24" s="5"/>
@@ -1634,66 +1645,66 @@
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" t="s">
         <v>41</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>42</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28" t="s">
         <v>43</v>
-      </c>
-      <c r="D28" t="s">
-        <v>44</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>23</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G28" s="8"/>
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>23</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G29" s="8"/>
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D31" s="5" t="s">
         <v>23</v>
@@ -1708,23 +1719,29 @@
     </row>
     <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B32" t="s">
-        <v>90</v>
+        <v>88</v>
+      </c>
+      <c r="C32" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B33" t="s">
-        <v>91</v>
+        <v>89</v>
+      </c>
+      <c r="C33" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B34" t="s">
         <v>13</v>
@@ -1748,10 +1765,10 @@
     <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C38" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
100% Tableau mis a jour
le mettre en francais :)
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fred/Desktop/OpenClassRoom/P4 Vrac/ProjetP4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C00701-F6DD-A24B-B6DC-4A4855B508E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4113687-49FD-F748-B090-4E925029538D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3100" yWindow="4780" windowWidth="46880" windowHeight="19880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="102">
   <si>
     <t>Catégorie</t>
   </si>
@@ -325,6 +325,18 @@
   </si>
   <si>
     <t>Je les ai viré aucun rapport et blackHat</t>
+  </si>
+  <si>
+    <t>label mal placé</t>
+  </si>
+  <si>
+    <t>rajuot du focus</t>
+  </si>
+  <si>
+    <t>rajout du aria label sur icones sociaux</t>
+  </si>
+  <si>
+    <t>aria label sur le skiplink</t>
   </si>
 </sst>
 </file>
@@ -1137,7 +1149,7 @@
   <dimension ref="A1:Z1018"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1774,10 +1786,26 @@
     <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C42" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C43" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C44" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C45" t="s">
+        <v>101</v>
+      </c>
+    </row>
     <row r="46" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="47" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Fred 100% Tableau avance
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fred/Desktop/OpenClassRoom/P4 Vrac/ProjetP4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4113687-49FD-F748-B090-4E925029538D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{045DFEF2-4E9B-F041-A5BD-99BF4177B80E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3100" yWindow="4780" windowWidth="46880" windowHeight="19880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,10 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="102">
-  <si>
-    <t>Catégorie</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="105">
   <si>
     <t>Problème identifié</t>
   </si>
@@ -51,18 +48,12 @@
     <t>Référence</t>
   </si>
   <si>
-    <t>(SEO ou accessiblité ?)</t>
-  </si>
-  <si>
     <t>SEO</t>
   </si>
   <si>
     <t>Balise Title</t>
   </si>
   <si>
-    <t>il faut que google connaise le titre de la page c'est le minimum</t>
-  </si>
-  <si>
     <t>en mettre une</t>
   </si>
   <si>
@@ -84,48 +75,24 @@
     <t>Balise Description content</t>
   </si>
   <si>
-    <t>c'est ce qui est afffiché pour les résultats</t>
-  </si>
-  <si>
     <t>bien chercher les mots clés</t>
   </si>
   <si>
-    <t>le faire en mode naturel pour l'utilisateur mais aussi avec en premier les mots google importants</t>
-  </si>
-  <si>
     <t>Page2</t>
   </si>
   <si>
-    <t>cela ne veut rien dire</t>
-  </si>
-  <si>
-    <t>trouver un nom de page exemple contact</t>
-  </si>
-  <si>
     <t>le faire</t>
   </si>
   <si>
     <t>Keyword</t>
   </si>
   <si>
-    <t>la virer</t>
-  </si>
-  <si>
-    <t>seo</t>
-  </si>
-  <si>
-    <t>texte blanc sur fond blanc</t>
-  </si>
-  <si>
     <t>a virer</t>
   </si>
   <si>
     <t>dans footer et dans le header</t>
   </si>
   <si>
-    <t>sEO</t>
-  </si>
-  <si>
     <t>image trop lourdes</t>
   </si>
   <si>
@@ -153,9 +120,6 @@
     <t>mettre lyon et meilleurs description</t>
   </si>
   <si>
-    <t>accesibilité</t>
-  </si>
-  <si>
     <t>Taille trop petite</t>
   </si>
   <si>
@@ -279,9 +243,6 @@
     <t>le recadrer</t>
   </si>
   <si>
-    <t>X</t>
-  </si>
-  <si>
     <t>Menu Accueil version desktop</t>
   </si>
   <si>
@@ -303,21 +264,12 @@
     <t>alt contenait paris</t>
   </si>
   <si>
-    <t>liens partenraire blackhat</t>
-  </si>
-  <si>
     <t>installer l'extension chrome wave</t>
   </si>
   <si>
     <t>Lien Wave</t>
   </si>
   <si>
-    <t>Agence web à paris, stratégie web, web design, illustrations, des…..</t>
-  </si>
-  <si>
-    <t>BlackHat  considérer comme une tentative de mauvais referement et se faire allumer</t>
-  </si>
-  <si>
     <t>Je l'ai viré on est a Lyon</t>
   </si>
   <si>
@@ -337,42 +289,74 @@
   </si>
   <si>
     <t>aria label sur le skiplink</t>
+  </si>
+  <si>
+    <t>liens  partenaires n'ont aucun rapport</t>
+  </si>
+  <si>
+    <t>CAT</t>
+  </si>
+  <si>
+    <t>Accesibilité</t>
+  </si>
+  <si>
+    <t>Lien caché BlackHat</t>
+  </si>
+  <si>
+    <t>Mettre une vrai balise avec une bonne recherche de mots clés</t>
+  </si>
+  <si>
+    <t>Mettre une vrai balise KeyWord</t>
+  </si>
+  <si>
+    <t>Affiché pour les résultats de recherche Google</t>
+  </si>
+  <si>
+    <t>Page2 ne veut rien dire cela n'aide pas au référencement</t>
+  </si>
+  <si>
+    <t>Mettre un title qui correspond a la page</t>
+  </si>
+  <si>
+    <t>Renommer la Page2 en Contact.html</t>
+  </si>
+  <si>
+    <t>Google a besoin de la la langue pour mieux indexer</t>
+  </si>
+  <si>
+    <t>&lt;html lang=""&gt;</t>
+  </si>
+  <si>
+    <t>Mettre la langue du site</t>
+  </si>
+  <si>
+    <t>Mettre la balise en &lt;html lang="fr"&gt;</t>
+  </si>
+  <si>
+    <t>Google ne connait pas la langue</t>
+  </si>
+  <si>
+    <t>Mode naturel et mettre les mots google importants</t>
+  </si>
+  <si>
+    <t>OpenClassRooms</t>
+  </si>
+  <si>
+    <t>Texte blanc/Fond blanc</t>
+  </si>
+  <si>
+    <t>Texte caché encore BlackHat + Paris alors que c'est Lyon</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="12"/>
@@ -388,15 +372,35 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="12"/>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
       <color theme="3"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="14"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
-      <color rgb="FFFF0000"/>
+      <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -433,35 +437,84 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="9">
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -474,7 +527,7 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="12"/>
+        <sz val="14"/>
         <color rgb="FFFFFFFF"/>
         <name val="Arial"/>
         <family val="2"/>
@@ -487,6 +540,54 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -507,7 +608,7 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>4603750</xdr:colOff>
-      <xdr:row>38</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4464050" cy="749300"/>
@@ -933,18 +1034,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E796EE32-1DFE-CD45-A2AF-F728FFC58B5F}" name="Tableau1" displayName="Tableau1" ref="A1:G38" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:G38" xr:uid="{E796EE32-1DFE-CD45-A2AF-F728FFC58B5F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E796EE32-1DFE-CD45-A2AF-F728FFC58B5F}" name="Tableau1" displayName="Tableau1" ref="A1:G36" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:G36" xr:uid="{E796EE32-1DFE-CD45-A2AF-F728FFC58B5F}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{9BB85078-D1DA-EA4F-939E-EA2B94AC6A91}" name="Catégorie"/>
-    <tableColumn id="2" xr3:uid="{701895DD-CBC8-C945-8BB8-1AF30E309D3E}" name="Problème identifié"/>
-    <tableColumn id="3" xr3:uid="{8B278B00-9A53-D541-81DA-33000B0C5DCC}" name="Explication du problème"/>
-    <tableColumn id="4" xr3:uid="{4C6455B9-1BC5-7D47-B3D3-56985A6D57BE}" name="Bonne pratique à adopter"/>
-    <tableColumn id="5" xr3:uid="{D4090782-153B-B745-8747-522ACAF6A5EB}" name="Action recommandée"/>
-    <tableColumn id="6" xr3:uid="{7DD18BAA-95ED-C642-8863-3D6C66C78033}" name="Référence"/>
-    <tableColumn id="7" xr3:uid="{0B8FBB93-CD44-6B49-B0E8-50644C7F0099}" name="OK ?" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{9BB85078-D1DA-EA4F-939E-EA2B94AC6A91}" name="CAT" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{701895DD-CBC8-C945-8BB8-1AF30E309D3E}" name="Problème identifié" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{8B278B00-9A53-D541-81DA-33000B0C5DCC}" name="Explication du problème" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{4C6455B9-1BC5-7D47-B3D3-56985A6D57BE}" name="Bonne pratique à adopter" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{D4090782-153B-B745-8747-522ACAF6A5EB}" name="Action recommandée" dataDxfId="2"/>
+    <tableColumn id="6" xr3:uid="{7DD18BAA-95ED-C642-8863-3D6C66C78033}" name="Référence" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{0B8FBB93-CD44-6B49-B0E8-50644C7F0099}" name="OK ?" dataDxfId="1"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -1146,666 +1247,717 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1018"/>
+  <dimension ref="A1:Z1016"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="66.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="70.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.28515625" style="9" bestFit="1" customWidth="1"/>
-    <col min="8" max="27" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="40.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="62.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="79.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="27" width="10.5703125" style="1" customWidth="1"/>
+    <col min="28" max="16384" width="11.28515625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="9"/>
+    </row>
+    <row r="2" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="B2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="E3" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="F4" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="E5" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="F5" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="4"/>
+    </row>
+    <row r="9" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="4"/>
+    </row>
+    <row r="10" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G10" s="4"/>
+    </row>
+    <row r="11" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="4"/>
+    </row>
+    <row r="12" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" s="4"/>
+    </row>
+    <row r="13" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="10"/>
+      <c r="F16" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G16" s="4"/>
+    </row>
+    <row r="17" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G17" s="4"/>
+    </row>
+    <row r="18" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G18" s="4"/>
+    </row>
+    <row r="19" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="D19" s="5"/>
+      <c r="E19" s="10"/>
+      <c r="F19" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G19" s="4"/>
+    </row>
+    <row r="20" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G20" s="4"/>
+    </row>
+    <row r="21" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" s="5"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="4"/>
+    </row>
+    <row r="22" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D22" s="5"/>
+      <c r="E22" s="10"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+    </row>
+    <row r="23" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="4"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="10"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+    </row>
+    <row r="24" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G24" s="4"/>
+    </row>
+    <row r="25" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="G25" s="4"/>
+    </row>
+    <row r="26" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="4"/>
+    </row>
+    <row r="27" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="G27" s="4"/>
+    </row>
+    <row r="28" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="4"/>
+    </row>
+    <row r="29" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2"/>
-      <c r="U1" s="2"/>
-      <c r="V1" s="2"/>
-      <c r="W1" s="2"/>
-      <c r="X1" s="2"/>
-      <c r="Y1" s="2"/>
-      <c r="Z1" s="2"/>
-    </row>
-    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2" s="4"/>
-      <c r="G2" s="8"/>
-    </row>
-    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="C29" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+    </row>
+    <row r="30" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F30" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" s="8" t="s">
+      <c r="G30" s="4"/>
+    </row>
+    <row r="31" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="4"/>
+    </row>
+    <row r="32" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="10"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="4"/>
+    </row>
+    <row r="33" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="4"/>
+    </row>
+    <row r="34" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="4"/>
+    </row>
+    <row r="35" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="4"/>
+    </row>
+    <row r="36" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="5"/>
+      <c r="B36" s="5"/>
+      <c r="C36" s="5" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" s="8"/>
-    </row>
-    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>17</v>
-      </c>
-      <c r="D5" t="s">
-        <v>18</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="10" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" s="8"/>
-    </row>
-    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" t="s">
-        <v>94</v>
-      </c>
-      <c r="D7" t="s">
-        <v>25</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="8"/>
-    </row>
-    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="D8" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="F8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="8"/>
-    </row>
-    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>30</v>
-      </c>
-      <c r="B9" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="D9" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" t="s">
-        <v>33</v>
-      </c>
-      <c r="G9" s="8"/>
-    </row>
-    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="D10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" s="8"/>
-    </row>
-    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11" t="s">
-        <v>36</v>
-      </c>
-      <c r="C11" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="D11" t="s">
-        <v>37</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" s="8"/>
-    </row>
-    <row r="12" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="D12" t="s">
-        <v>39</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" s="8"/>
-    </row>
-    <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B13" t="s">
-        <v>44</v>
-      </c>
-      <c r="C13" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="4"/>
-      <c r="F13" t="s">
-        <v>47</v>
-      </c>
-      <c r="G13" s="8"/>
-    </row>
-    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C14" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="G14" s="8"/>
-    </row>
-    <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>7</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="F15" t="s">
-        <v>47</v>
-      </c>
-      <c r="G15" s="8"/>
-    </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B17" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="C17" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>50</v>
-      </c>
-      <c r="G17" s="8"/>
-    </row>
-    <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D18" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="E18" s="4"/>
-      <c r="F18" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="G18" s="8"/>
-    </row>
-    <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="C19" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D19" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="G19" s="8"/>
-    </row>
-    <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B20" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D20" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="G20" s="8"/>
-    </row>
-    <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B21" s="5" t="s">
+      <c r="D36" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="G21" s="8"/>
-    </row>
-    <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D22" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>63</v>
-      </c>
-      <c r="G22" s="8"/>
-    </row>
-    <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="D23" s="5"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="5"/>
-      <c r="G23" s="8"/>
-    </row>
-    <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="5"/>
-      <c r="B24" t="s">
-        <v>90</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="D24" s="5"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="8"/>
-    </row>
-    <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="5"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="5"/>
-      <c r="G25" s="8"/>
-    </row>
-    <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="8"/>
-    </row>
-    <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E27" s="4"/>
-      <c r="G27" s="8"/>
-    </row>
-    <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>40</v>
-      </c>
-      <c r="B28" t="s">
-        <v>41</v>
-      </c>
-      <c r="C28" t="s">
-        <v>42</v>
-      </c>
-      <c r="D28" t="s">
-        <v>43</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="G28" s="8"/>
-    </row>
-    <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>40</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="D29" s="5" t="s">
-        <v>71</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="G29" s="8"/>
-    </row>
-    <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>40</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C30" s="5" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>40</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="C31" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="F31" t="s">
-        <v>12</v>
-      </c>
-      <c r="G31" s="8"/>
-    </row>
-    <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>40</v>
-      </c>
-      <c r="B32" t="s">
-        <v>88</v>
-      </c>
-      <c r="C32" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>40</v>
-      </c>
-      <c r="B33" t="s">
-        <v>89</v>
-      </c>
-      <c r="C33" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>40</v>
-      </c>
-      <c r="B34" t="s">
-        <v>13</v>
-      </c>
-      <c r="C34" t="s">
-        <v>14</v>
-      </c>
-      <c r="D34" t="s">
-        <v>15</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F34" t="s">
-        <v>12</v>
-      </c>
-      <c r="G34" s="8"/>
-    </row>
-    <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="4"/>
+    </row>
     <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C38" t="s">
-        <v>91</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>92</v>
-      </c>
-    </row>
+    <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C42" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C43" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C44" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C45" t="s">
-        <v>101</v>
-      </c>
-    </row>
+    <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="46" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="47" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2777,19 +2929,19 @@
     <row r="1014" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1015" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1016" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1017" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1018" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C11" r:id="rId1" display="https://fredericguilet.github.io/P4Guillet_Frederic25072021/voiture.com" xr:uid="{F0E0A3CD-37FD-9E44-B979-49DC1760F2BE}"/>
-    <hyperlink ref="C12" r:id="rId2" display="https://fredericguilet.github.io/P4Guillet_Frederic25072021/pizza.com" xr:uid="{68CF73CC-7EFC-0048-B22E-4CE39E7A4D9F}"/>
-    <hyperlink ref="D38" r:id="rId3" xr:uid="{8B9623D5-26B1-F54A-9395-E5EC71494DBA}"/>
+    <hyperlink ref="C10" r:id="rId1" display="https://fredericguilet.github.io/P4Guillet_Frederic25072021/voiture.com" xr:uid="{F0E0A3CD-37FD-9E44-B979-49DC1760F2BE}"/>
+    <hyperlink ref="C11" r:id="rId2" display="https://fredericguilet.github.io/P4Guillet_Frederic25072021/pizza.com" xr:uid="{68CF73CC-7EFC-0048-B22E-4CE39E7A4D9F}"/>
+    <hyperlink ref="D36" r:id="rId3" xr:uid="{8B9623D5-26B1-F54A-9395-E5EC71494DBA}"/>
+    <hyperlink ref="F2" r:id="rId4" xr:uid="{DF56BA83-E4D7-3D49-8E46-5DA1D7F0BF6B}"/>
+    <hyperlink ref="F3:F6" r:id="rId5" display="OpenClassRooms" xr:uid="{FBEF5557-F283-B44B-8AD5-18C42F6301B5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId4"/>
+  <drawing r:id="rId6"/>
   <tableParts count="1">
-    <tablePart r:id="rId5"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fred 100% MAJ TABLO
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fred/Desktop/OpenClassRoom/P4 Vrac/ProjetP4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{045DFEF2-4E9B-F041-A5BD-99BF4177B80E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4126586F-B030-E648-B1AC-4A9ADAD09D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3100" yWindow="4780" windowWidth="46880" windowHeight="19880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="110">
   <si>
     <t>Problème identifié</t>
   </si>
@@ -57,9 +57,6 @@
     <t>en mettre une</t>
   </si>
   <si>
-    <t xml:space="preserve">en mettre une </t>
-  </si>
-  <si>
     <t>open class room et du bon sens</t>
   </si>
   <si>
@@ -87,39 +84,6 @@
     <t>Keyword</t>
   </si>
   <si>
-    <t>a virer</t>
-  </si>
-  <si>
-    <t>dans footer et dans le header</t>
-  </si>
-  <si>
-    <t>image trop lourdes</t>
-  </si>
-  <si>
-    <t>mettre en webp</t>
-  </si>
-  <si>
-    <t>mon mentor</t>
-  </si>
-  <si>
-    <t>images taille exactes</t>
-  </si>
-  <si>
-    <t>les agggrandirs</t>
-  </si>
-  <si>
-    <t>Balise H1</t>
-  </si>
-  <si>
-    <t>il faut expliquer ce que fait l'agence</t>
-  </si>
-  <si>
-    <t>footer</t>
-  </si>
-  <si>
-    <t>mettre lyon et meilleurs description</t>
-  </si>
-  <si>
     <t>Taille trop petite</t>
   </si>
   <si>
@@ -129,9 +93,6 @@
     <t>mettre en plus gros les polices</t>
   </si>
   <si>
-    <t>robots follow</t>
-  </si>
-  <si>
     <t>contenus pas assez fourni</t>
   </si>
   <si>
@@ -189,24 +150,9 @@
     <t>moi-même</t>
   </si>
   <si>
-    <t>Partenaires</t>
-  </si>
-  <si>
     <t>500 mots au max</t>
   </si>
   <si>
-    <t>Pas  bonne trop basique</t>
-  </si>
-  <si>
-    <t>pas de localisation</t>
-  </si>
-  <si>
-    <t>le mettre en yes</t>
-  </si>
-  <si>
-    <t>probleme si brower a 120% les augementer</t>
-  </si>
-  <si>
     <t>moi je l'ais fait a l'époque pour les clients</t>
   </si>
   <si>
@@ -333,19 +279,88 @@
     <t>Mettre la balise en &lt;html lang="fr"&gt;</t>
   </si>
   <si>
-    <t>Google ne connait pas la langue</t>
-  </si>
-  <si>
     <t>Mode naturel et mettre les mots google importants</t>
   </si>
   <si>
     <t>OpenClassRooms</t>
   </si>
   <si>
-    <t>Texte blanc/Fond blanc</t>
-  </si>
-  <si>
     <t>Texte caché encore BlackHat + Paris alors que c'est Lyon</t>
+  </si>
+  <si>
+    <t>Texte blanc/Fond blanc Footer et Header</t>
+  </si>
+  <si>
+    <t>Ne pas le faire risque d'etre Blaklisté</t>
+  </si>
+  <si>
+    <t>Ne pas le faire</t>
+  </si>
+  <si>
+    <t>Image trop lourdes a charger</t>
+  </si>
+  <si>
+    <t>Images au lieu de texte exemple citation</t>
+  </si>
+  <si>
+    <t>Le site met du temps a charger les surfeurs risquent de partir</t>
+  </si>
+  <si>
+    <t>Mettre un format plus adapté</t>
+  </si>
+  <si>
+    <t>Changement en mode Webp plus légeres et pas de perte de qualité</t>
+  </si>
+  <si>
+    <t>Hugo Dumont</t>
+  </si>
+  <si>
+    <t>Les Images ont une taille exacte</t>
+  </si>
+  <si>
+    <t>Certains Browser peuvent mal les voir</t>
+  </si>
+  <si>
+    <t>Mettre un format légerement plus grand</t>
+  </si>
+  <si>
+    <t>Pas de balise Titile mauvais indéxation</t>
+  </si>
+  <si>
+    <t>Mettre une balise Title explicite</t>
+  </si>
+  <si>
+    <t>Mettre title en Accueil par exemple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Balise H1 </t>
+  </si>
+  <si>
+    <t>Dans les résultats de Google ce que les gens peuvent voir</t>
+  </si>
+  <si>
+    <t>Mettre une phrase pour google pour une meilleur indexation mais aussi en francais pour les surfeurs</t>
+  </si>
+  <si>
+    <t>Balise Footer</t>
+  </si>
+  <si>
+    <t>Pas de localisation indiquée</t>
+  </si>
+  <si>
+    <t>La localisation sert a mieux se positionner pour ceux qui ont indiqués ce mot clé</t>
+  </si>
+  <si>
+    <t>Robots follow</t>
+  </si>
+  <si>
+    <t>Le Robot de Google ne va qu'indexer la premiere page</t>
+  </si>
+  <si>
+    <t>Mettre le follow en yes</t>
+  </si>
+  <si>
+    <t>Cela permet de mieux suivre les autres liens du site</t>
   </si>
 </sst>
 </file>
@@ -608,7 +623,7 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>4603750</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>37</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4464050" cy="749300"/>
@@ -1034,8 +1049,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E796EE32-1DFE-CD45-A2AF-F728FFC58B5F}" name="Tableau1" displayName="Tableau1" ref="A1:G36" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:G36" xr:uid="{E796EE32-1DFE-CD45-A2AF-F728FFC58B5F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E796EE32-1DFE-CD45-A2AF-F728FFC58B5F}" name="Tableau1" displayName="Tableau1" ref="A1:G37" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:G37" xr:uid="{E796EE32-1DFE-CD45-A2AF-F728FFC58B5F}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{9BB85078-D1DA-EA4F-939E-EA2B94AC6A91}" name="CAT" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{701895DD-CBC8-C945-8BB8-1AF30E309D3E}" name="Problème identifié" dataDxfId="7"/>
@@ -1247,10 +1262,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1016"/>
+  <dimension ref="A1:Z1017"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1268,7 +1283,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>87</v>
+        <v>69</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -1286,7 +1301,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>64</v>
+        <v>46</v>
       </c>
       <c r="H1" s="9"/>
       <c r="I1" s="9"/>
@@ -1316,19 +1331,19 @@
         <v>6</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>7</v>
+        <v>98</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>8</v>
+        <v>99</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -1336,22 +1351,22 @@
         <v>5</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>97</v>
+        <v>79</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -1359,22 +1374,22 @@
         <v>5</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>14</v>
-      </c>
       <c r="E4" s="10" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -1382,22 +1397,22 @@
         <v>5</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>93</v>
+        <v>75</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>95</v>
+        <v>77</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -1405,22 +1420,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>89</v>
+        <v>71</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>91</v>
+        <v>73</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>90</v>
+        <v>72</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>65</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -1428,122 +1443,130 @@
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>18</v>
+        <v>86</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" s="4"/>
+        <v>87</v>
+      </c>
+      <c r="F7" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="8" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>20</v>
+        <v>88</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>52</v>
+        <v>90</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>21</v>
+        <v>91</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G8" s="4"/>
+        <v>92</v>
+      </c>
+      <c r="F8" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="9" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>23</v>
+        <v>94</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>57</v>
+        <v>95</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" s="4"/>
+        <v>96</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="F9" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="10" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>25</v>
+        <v>100</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>54</v>
+        <v>101</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E10" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="4"/>
+        <v>102</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="11" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>27</v>
+        <v>103</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>55</v>
+        <v>104</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="E11" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G11" s="4"/>
+        <v>105</v>
+      </c>
+      <c r="E11" s="10"/>
+      <c r="F11" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>47</v>
+      </c>
     </row>
     <row r="12" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>32</v>
+        <v>106</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>56</v>
+        <v>107</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="10"/>
+        <v>108</v>
+      </c>
+      <c r="E12" s="10" t="s">
+        <v>109</v>
+      </c>
       <c r="F12" s="4" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="G12" s="4"/>
     </row>
@@ -1552,19 +1575,19 @@
         <v>5</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F13" s="4" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="G13" s="4"/>
     </row>
@@ -1573,19 +1596,19 @@
         <v>5</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>58</v>
+        <v>40</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="G14" s="4"/>
     </row>
@@ -1594,16 +1617,16 @@
         <v>5</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="F15" s="4"/>
       <c r="G15" s="4"/>
@@ -1613,17 +1636,17 @@
         <v>5</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="E16" s="10"/>
       <c r="F16" s="4" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="G16" s="4"/>
     </row>
@@ -1632,19 +1655,19 @@
         <v>5</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="G17" s="4"/>
     </row>
@@ -1653,19 +1676,19 @@
         <v>5</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>61</v>
+        <v>43</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="D18" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>63</v>
+        <v>45</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="G18" s="4"/>
     </row>
@@ -1674,15 +1697,15 @@
         <v>5</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
       <c r="D19" s="5"/>
       <c r="E19" s="10"/>
       <c r="F19" s="4" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="G19" s="4"/>
     </row>
@@ -1691,19 +1714,19 @@
         <v>5</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>70</v>
+        <v>52</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>68</v>
+        <v>50</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>69</v>
+        <v>51</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="G20" s="4"/>
     </row>
@@ -1712,10 +1735,10 @@
         <v>5</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>71</v>
+        <v>53</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="D21" s="5"/>
       <c r="E21" s="10"/>
@@ -1727,127 +1750,125 @@
         <v>5</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>81</v>
-      </c>
+        <v>89</v>
+      </c>
+      <c r="C22" s="5"/>
       <c r="D22" s="5"/>
       <c r="E22" s="10"/>
       <c r="F22" s="4"/>
       <c r="G22" s="4"/>
     </row>
     <row r="23" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="4"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
+      <c r="A23" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>63</v>
+      </c>
       <c r="D23" s="5"/>
       <c r="E23" s="10"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
     </row>
     <row r="24" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>47</v>
-      </c>
+      <c r="A24" s="4"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="10"/>
+      <c r="F24" s="4"/>
       <c r="G24" s="4"/>
     </row>
     <row r="25" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>36</v>
+        <v>17</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>39</v>
+        <v>18</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="G25" s="4"/>
     </row>
     <row r="26" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>73</v>
+        <v>23</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="4"/>
+        <v>26</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="G26" s="4"/>
     </row>
     <row r="27" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E27" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>9</v>
-      </c>
+        <v>55</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="4"/>
       <c r="G27" s="4"/>
     </row>
     <row r="28" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C28" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="4"/>
+        <v>27</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="G28" s="4"/>
     </row>
     <row r="29" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
@@ -1856,44 +1877,46 @@
     </row>
     <row r="30" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>9</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="4"/>
       <c r="G30" s="4"/>
     </row>
     <row r="31" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>8</v>
+      </c>
       <c r="G31" s="4"/>
     </row>
     <row r="32" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -1903,23 +1926,23 @@
     </row>
     <row r="33" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
+      <c r="E33" s="10"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
     </row>
     <row r="34" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>88</v>
+        <v>70</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -1928,8 +1951,12 @@
       <c r="G34" s="4"/>
     </row>
     <row r="35" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="5"/>
-      <c r="B35" s="5"/>
+      <c r="A35" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>67</v>
+      </c>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
@@ -1939,17 +1966,25 @@
     <row r="36" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
-      <c r="C36" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>78</v>
-      </c>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
       <c r="E36" s="5"/>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
     </row>
-    <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="5"/>
+      <c r="B37" s="5"/>
+      <c r="C37" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="E37" s="5"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="4"/>
+    </row>
     <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2929,19 +2964,25 @@
     <row r="1014" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1015" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1016" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1017" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C10" r:id="rId1" display="https://fredericguilet.github.io/P4Guillet_Frederic25072021/voiture.com" xr:uid="{F0E0A3CD-37FD-9E44-B979-49DC1760F2BE}"/>
     <hyperlink ref="C11" r:id="rId2" display="https://fredericguilet.github.io/P4Guillet_Frederic25072021/pizza.com" xr:uid="{68CF73CC-7EFC-0048-B22E-4CE39E7A4D9F}"/>
-    <hyperlink ref="D36" r:id="rId3" xr:uid="{8B9623D5-26B1-F54A-9395-E5EC71494DBA}"/>
+    <hyperlink ref="D37" r:id="rId3" xr:uid="{8B9623D5-26B1-F54A-9395-E5EC71494DBA}"/>
     <hyperlink ref="F2" r:id="rId4" xr:uid="{DF56BA83-E4D7-3D49-8E46-5DA1D7F0BF6B}"/>
     <hyperlink ref="F3:F6" r:id="rId5" display="OpenClassRooms" xr:uid="{FBEF5557-F283-B44B-8AD5-18C42F6301B5}"/>
+    <hyperlink ref="F7" r:id="rId6" xr:uid="{210A7551-794E-B34C-AA75-9FCA644AE40B}"/>
+    <hyperlink ref="F8" r:id="rId7" xr:uid="{140B208B-D31E-214A-A1BB-CDC3896E4F8F}"/>
+    <hyperlink ref="F9" r:id="rId8" xr:uid="{1CAF9DA3-EF35-E54A-87AB-439617F277AE}"/>
+    <hyperlink ref="F10" r:id="rId9" xr:uid="{ECC056D8-7AF8-064A-B011-2942CAFE8449}"/>
+    <hyperlink ref="F11" r:id="rId10" xr:uid="{9841D446-7B53-634A-883A-63FC63860DF9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId6"/>
+  <drawing r:id="rId11"/>
   <tableParts count="1">
-    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId12"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fred 100% Tablo avance bien
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fred/Desktop/OpenClassRoom/P4 Vrac/ProjetP4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4126586F-B030-E648-B1AC-4A9ADAD09D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EEC18D8-7F35-D847-B76B-5DD6CD3F52EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3100" yWindow="4780" windowWidth="46880" windowHeight="19880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="116">
   <si>
     <t>Problème identifié</t>
   </si>
@@ -54,9 +54,6 @@
     <t>Balise Title</t>
   </si>
   <si>
-    <t>en mettre une</t>
-  </si>
-  <si>
     <t>open class room et du bon sens</t>
   </si>
   <si>
@@ -93,24 +90,12 @@
     <t>mettre en plus gros les polices</t>
   </si>
   <si>
-    <t>contenus pas assez fourni</t>
-  </si>
-  <si>
     <t>Checklist #SEO</t>
   </si>
   <si>
-    <t>experience perso</t>
-  </si>
-  <si>
     <t>balise alt sur les images</t>
   </si>
   <si>
-    <t>copyright dans les images</t>
-  </si>
-  <si>
-    <t>pas le faire mentor m'as indiqué que c'est peanuts</t>
-  </si>
-  <si>
     <t>pour savoir ce que représent l'image</t>
   </si>
   <si>
@@ -120,57 +105,18 @@
     <t>Questions Réponses</t>
   </si>
   <si>
-    <t>en mettre car recherche sous goole = soucent des questions</t>
-  </si>
-  <si>
-    <t>le faire ?</t>
-  </si>
-  <si>
     <t>BootStrap</t>
   </si>
   <si>
-    <t>pas a jour probleme de vulnartibilité</t>
-  </si>
-  <si>
-    <t>lighthouse</t>
-  </si>
-  <si>
     <t>Checklist #SEO et lighthouse</t>
   </si>
   <si>
-    <t>Page formulaire</t>
-  </si>
-  <si>
-    <t>pourquoi en anglais les erreurs</t>
-  </si>
-  <si>
-    <t>mettre en frances</t>
-  </si>
-  <si>
-    <t>moi-même</t>
-  </si>
-  <si>
-    <t>500 mots au max</t>
-  </si>
-  <si>
-    <t>moi je l'ais fait a l'époque pour les clients</t>
-  </si>
-  <si>
     <t>Mettre les balises alt</t>
   </si>
   <si>
     <t>footer ectc en remarques</t>
   </si>
   <si>
-    <t>htacsess pour les erreurs 404 par exemple</t>
-  </si>
-  <si>
-    <t>utilisateur paumé</t>
-  </si>
-  <si>
-    <t>avec ou sans javasript ?</t>
-  </si>
-  <si>
     <t>OK ?</t>
   </si>
   <si>
@@ -180,22 +126,7 @@
     <t>Commentaires en images</t>
   </si>
   <si>
-    <t>pourquoi</t>
-  </si>
-  <si>
-    <t>il sort du cadre</t>
-  </si>
-  <si>
-    <t>le recadrer</t>
-  </si>
-  <si>
-    <t>Menu Accueil version desktop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Navbar header </t>
-  </si>
-  <si>
-    <t>contient les keyword en mode caché</t>
+    <t>X</t>
   </si>
   <si>
     <t>Changement couleur</t>
@@ -222,9 +153,6 @@
     <t>changé en ombre plus propre</t>
   </si>
   <si>
-    <t>Je les ai viré aucun rapport et blackHat</t>
-  </si>
-  <si>
     <t>label mal placé</t>
   </si>
   <si>
@@ -237,9 +165,6 @@
     <t>aria label sur le skiplink</t>
   </si>
   <si>
-    <t>liens  partenaires n'ont aucun rapport</t>
-  </si>
-  <si>
     <t>CAT</t>
   </si>
   <si>
@@ -300,9 +225,6 @@
     <t>Image trop lourdes a charger</t>
   </si>
   <si>
-    <t>Images au lieu de texte exemple citation</t>
-  </si>
-  <si>
     <t>Le site met du temps a charger les surfeurs risquent de partir</t>
   </si>
   <si>
@@ -361,13 +283,109 @@
   </si>
   <si>
     <t>Cela permet de mieux suivre les autres liens du site</t>
+  </si>
+  <si>
+    <t>Contenus pas assez fourni</t>
+  </si>
+  <si>
+    <t>Le faire a l'occasion en parler a la direction</t>
+  </si>
+  <si>
+    <t>Copyright dans les images</t>
+  </si>
+  <si>
+    <t>Peut servir si le surfeur cherche par images sous Google</t>
+  </si>
+  <si>
+    <t>Pas obligatoire</t>
+  </si>
+  <si>
+    <t>Le faire ou pas à  l'occasion en parler a la direction</t>
+  </si>
+  <si>
+    <t>Pas de FAQ ou de questions réponses pour les futurs clients</t>
+  </si>
+  <si>
+    <t>Certains sous Google cherchent par question</t>
+  </si>
+  <si>
+    <t>Réflexion Personnelle</t>
+  </si>
+  <si>
+    <t>JSQuery</t>
+  </si>
+  <si>
+    <t>Probleme de Vulnérabilité Version Ancienne</t>
+  </si>
+  <si>
+    <t>Toujours bien mettre a jour les outils utilisés</t>
+  </si>
+  <si>
+    <t>Le faire absolument en parler a la direction</t>
+  </si>
+  <si>
+    <t>LightHouse</t>
+  </si>
+  <si>
+    <t>Le faire absolument  Sparadra un petit script dans page contact en attendant</t>
+  </si>
+  <si>
+    <t>Formulaire dans page Contact</t>
+  </si>
+  <si>
+    <t>Les Erreurs sont en anglais</t>
+  </si>
+  <si>
+    <t>Mettre dans la langue d'origine</t>
+  </si>
+  <si>
+    <t>htacsess pour Erreurs 404 etc</t>
+  </si>
+  <si>
+    <t>Si la personne tape un mauvais lien il se trouve devant une page d'erreur</t>
+  </si>
+  <si>
+    <t>Certaines images peuvent se remplacer par du texte</t>
+  </si>
+  <si>
+    <t>Quand pas besoin d'image mettre du texte</t>
+  </si>
+  <si>
+    <t>Le faire les  citations ou avis clients dont rès recherchées par Google</t>
+  </si>
+  <si>
+    <t>Menu Contact Version Desktop</t>
+  </si>
+  <si>
+    <t>Le Menu sort du cadre difficile de surfer</t>
+  </si>
+  <si>
+    <t>Le lien Css n'est pas le meme que l'accueil</t>
+  </si>
+  <si>
+    <t>Mettre le meme lien css que le menu principal pour éviter des surprises</t>
+  </si>
+  <si>
+    <t>Les liens  partenaires n'ont aucun rapport</t>
+  </si>
+  <si>
+    <t>Mettre des Liens cohérents avec le sujet</t>
+  </si>
+  <si>
+    <t>Mettre en place des stratégies partenaires de liens en parler a la direction</t>
+  </si>
+  <si>
+    <t>Contenus plus de 500 mots voire encore plus longs la longueur du texte compte pour référencement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Risque d'etre Blacklisté par Google anciennes pratiques  pas ok </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -396,6 +414,13 @@
     <font>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -454,7 +479,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -467,12 +492,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -623,7 +651,7 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>4603750</xdr:colOff>
-      <xdr:row>37</xdr:row>
+      <xdr:row>36</xdr:row>
       <xdr:rowOff>63500</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4464050" cy="749300"/>
@@ -1049,8 +1077,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E796EE32-1DFE-CD45-A2AF-F728FFC58B5F}" name="Tableau1" displayName="Tableau1" ref="A1:G37" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:G37" xr:uid="{E796EE32-1DFE-CD45-A2AF-F728FFC58B5F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E796EE32-1DFE-CD45-A2AF-F728FFC58B5F}" name="Tableau1" displayName="Tableau1" ref="A1:G36" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:G36" xr:uid="{E796EE32-1DFE-CD45-A2AF-F728FFC58B5F}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{9BB85078-D1DA-EA4F-939E-EA2B94AC6A91}" name="CAT" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{701895DD-CBC8-C945-8BB8-1AF30E309D3E}" name="Problème identifié" dataDxfId="7"/>
@@ -1262,19 +1290,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1017"/>
+  <dimension ref="A1:Z1016"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.140625" style="1" customWidth="1"/>
     <col min="2" max="2" width="40.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="62.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="79.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="68.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="44.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="82.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="27" width="10.5703125" style="1" customWidth="1"/>
@@ -1283,7 +1311,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -1301,7 +1329,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="H1" s="9"/>
       <c r="I1" s="9"/>
@@ -1331,19 +1359,19 @@
         <v>6</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>97</v>
+        <v>71</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>99</v>
+        <v>73</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -1351,22 +1379,22 @@
         <v>5</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>79</v>
+        <v>54</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>78</v>
+        <v>53</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>80</v>
+        <v>55</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>81</v>
+        <v>56</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -1374,22 +1402,22 @@
         <v>5</v>
       </c>
       <c r="B4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>13</v>
-      </c>
       <c r="E4" s="10" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -1397,22 +1425,22 @@
         <v>5</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>75</v>
+        <v>50</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>76</v>
+        <v>51</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>77</v>
+        <v>52</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -1420,22 +1448,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>71</v>
+        <v>46</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>72</v>
+        <v>47</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -1443,22 +1471,22 @@
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>85</v>
+        <v>60</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>84</v>
+        <v>59</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>87</v>
+        <v>62</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -1466,22 +1494,22 @@
         <v>5</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>88</v>
+        <v>63</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>91</v>
+        <v>65</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>92</v>
+        <v>66</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>93</v>
+        <v>67</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -1489,22 +1517,22 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>94</v>
+        <v>68</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>93</v>
+        <v>67</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -1512,20 +1540,20 @@
         <v>5</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>100</v>
+        <v>74</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>101</v>
+        <v>75</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>102</v>
+        <v>76</v>
       </c>
       <c r="E10" s="10"/>
       <c r="F10" s="11" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -1533,20 +1561,20 @@
         <v>5</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>103</v>
+        <v>77</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>104</v>
+        <v>78</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>105</v>
+        <v>79</v>
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="11" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>47</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -1554,321 +1582,363 @@
         <v>5</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>106</v>
+        <v>80</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>107</v>
+        <v>81</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>108</v>
+        <v>82</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G12" s="4"/>
+        <v>83</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="13" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>20</v>
+        <v>84</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>30</v>
-      </c>
+        <v>114</v>
+      </c>
+      <c r="D13" s="5"/>
       <c r="E13" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G13" s="4"/>
+        <v>85</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="14" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>24</v>
+        <v>86</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>40</v>
+        <v>87</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>30</v>
+        <v>88</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="G14" s="4"/>
+        <v>89</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="15" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>15</v>
+        <v>23</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>91</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
+        <v>85</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="16" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="G16" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D16" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E16" s="10"/>
-      <c r="F16" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="G16" s="4"/>
     </row>
     <row r="17" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>36</v>
+        <v>93</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>94</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>15</v>
+        <v>95</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G17" s="4"/>
+        <v>98</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="18" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>43</v>
+        <v>99</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>44</v>
+        <v>100</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G18" s="4"/>
+        <v>101</v>
+      </c>
+      <c r="E18" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="19" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>48</v>
+        <v>102</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G19" s="4"/>
+        <v>103</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E19" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>50</v>
+        <v>104</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>15</v>
+        <v>105</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="G20" s="4"/>
+        <v>106</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="21" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>53</v>
+        <v>107</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="D21" s="5"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
+        <v>108</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="22" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>89</v>
-      </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
+        <v>111</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" s="12" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="23" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>63</v>
-      </c>
+      <c r="A23" s="4"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="10"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
     </row>
     <row r="24" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="4"/>
-      <c r="B24" s="5"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="4"/>
+      <c r="A24" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>25</v>
+      </c>
       <c r="G24" s="4"/>
     </row>
     <row r="25" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="G25" s="4"/>
     </row>
     <row r="26" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>34</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="4"/>
       <c r="G26" s="4"/>
     </row>
     <row r="27" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C27" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D27" s="5"/>
-      <c r="E27" s="5"/>
-      <c r="F27" s="4"/>
+        <v>22</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="G27" s="4"/>
     </row>
     <row r="28" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D28" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>8</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="4"/>
       <c r="G28" s="4"/>
     </row>
     <row r="29" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="D29" s="5"/>
       <c r="E29" s="5"/>
@@ -1877,46 +1947,44 @@
     </row>
     <row r="30" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>58</v>
+        <v>8</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="D30" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>7</v>
+      </c>
       <c r="G30" s="4"/>
     </row>
     <row r="31" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>8</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="10"/>
+      <c r="F31" s="4"/>
       <c r="G31" s="4"/>
     </row>
     <row r="32" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="C32" s="5"/>
       <c r="D32" s="5"/>
@@ -1926,23 +1994,23 @@
     </row>
     <row r="33" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>65</v>
+        <v>42</v>
       </c>
       <c r="C33" s="5"/>
       <c r="D33" s="5"/>
-      <c r="E33" s="10"/>
+      <c r="E33" s="5"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
     </row>
     <row r="34" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -1951,12 +2019,8 @@
       <c r="G34" s="4"/>
     </row>
     <row r="35" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>67</v>
-      </c>
+      <c r="A35" s="5"/>
+      <c r="B35" s="5"/>
       <c r="C35" s="5"/>
       <c r="D35" s="5"/>
       <c r="E35" s="5"/>
@@ -1966,25 +2030,17 @@
     <row r="36" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
-      <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
+      <c r="C36" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>37</v>
+      </c>
       <c r="E36" s="5"/>
       <c r="F36" s="4"/>
       <c r="G36" s="4"/>
     </row>
-    <row r="37" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>60</v>
-      </c>
-      <c r="E37" s="5"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
-    </row>
+    <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2964,12 +3020,11 @@
     <row r="1014" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1015" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1016" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1017" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C10" r:id="rId1" display="https://fredericguilet.github.io/P4Guillet_Frederic25072021/voiture.com" xr:uid="{F0E0A3CD-37FD-9E44-B979-49DC1760F2BE}"/>
     <hyperlink ref="C11" r:id="rId2" display="https://fredericguilet.github.io/P4Guillet_Frederic25072021/pizza.com" xr:uid="{68CF73CC-7EFC-0048-B22E-4CE39E7A4D9F}"/>
-    <hyperlink ref="D37" r:id="rId3" xr:uid="{8B9623D5-26B1-F54A-9395-E5EC71494DBA}"/>
+    <hyperlink ref="D36" r:id="rId3" xr:uid="{8B9623D5-26B1-F54A-9395-E5EC71494DBA}"/>
     <hyperlink ref="F2" r:id="rId4" xr:uid="{DF56BA83-E4D7-3D49-8E46-5DA1D7F0BF6B}"/>
     <hyperlink ref="F3:F6" r:id="rId5" display="OpenClassRooms" xr:uid="{FBEF5557-F283-B44B-8AD5-18C42F6301B5}"/>
     <hyperlink ref="F7" r:id="rId6" xr:uid="{210A7551-794E-B34C-AA75-9FCA644AE40B}"/>
@@ -2977,12 +3032,23 @@
     <hyperlink ref="F9" r:id="rId8" xr:uid="{1CAF9DA3-EF35-E54A-87AB-439617F277AE}"/>
     <hyperlink ref="F10" r:id="rId9" xr:uid="{ECC056D8-7AF8-064A-B011-2942CAFE8449}"/>
     <hyperlink ref="F11" r:id="rId10" xr:uid="{9841D446-7B53-634A-883A-63FC63860DF9}"/>
+    <hyperlink ref="F12" r:id="rId11" xr:uid="{FFA3C916-33BF-324A-B768-5845F53E3B1C}"/>
+    <hyperlink ref="F13" r:id="rId12" xr:uid="{B1BAF8CE-606D-0B4F-8428-237F8CD57312}"/>
+    <hyperlink ref="F14" r:id="rId13" xr:uid="{2BFE7964-3028-644D-945B-22C79D77C8CC}"/>
+    <hyperlink ref="F15" r:id="rId14" xr:uid="{9BB76B05-4769-6A4A-BFE9-AB49E1089187}"/>
+    <hyperlink ref="F16" r:id="rId15" xr:uid="{E6818DFB-78F2-D143-A048-0EDCA090BB9A}"/>
+    <hyperlink ref="F17" r:id="rId16" xr:uid="{BCB0B4D9-E802-A641-8202-DEF07D85A9DE}"/>
+    <hyperlink ref="F18" r:id="rId17" xr:uid="{D21035A4-8923-904D-AB29-B185D2CBCBA9}"/>
+    <hyperlink ref="F19" r:id="rId18" xr:uid="{9B5ED51E-C284-A849-8F3A-BB456B5C58A6}"/>
+    <hyperlink ref="F20" r:id="rId19" xr:uid="{9940974C-2DE6-C849-8FFF-E00D77703634}"/>
+    <hyperlink ref="F21" r:id="rId20" xr:uid="{1ECF8826-8E64-8C4D-A5C5-F3A4B120FC8A}"/>
+    <hyperlink ref="F22" r:id="rId21" xr:uid="{CCDE431B-14C3-8D46-8EAB-D188D8E8C8A5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId11"/>
+  <drawing r:id="rId22"/>
   <tableParts count="1">
-    <tablePart r:id="rId12"/>
+    <tablePart r:id="rId23"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fred 100% Tableau presque fini
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fred/Desktop/OpenClassRoom/P4 Vrac/ProjetP4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EEC18D8-7F35-D847-B76B-5DD6CD3F52EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077AEFDB-1CB6-1B45-99E6-540ACFB39F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3100" yWindow="4780" windowWidth="46880" windowHeight="19880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="131">
   <si>
     <t>Problème identifié</t>
   </si>
@@ -54,18 +54,6 @@
     <t>Balise Title</t>
   </si>
   <si>
-    <t>open class room et du bon sens</t>
-  </si>
-  <si>
-    <t>lang</t>
-  </si>
-  <si>
-    <t>google ne connait pas la langue</t>
-  </si>
-  <si>
-    <t>mettre fr</t>
-  </si>
-  <si>
     <t>Balise Description content</t>
   </si>
   <si>
@@ -75,48 +63,18 @@
     <t>Page2</t>
   </si>
   <si>
-    <t>le faire</t>
-  </si>
-  <si>
     <t>Keyword</t>
   </si>
   <si>
-    <t>Taille trop petite</t>
-  </si>
-  <si>
-    <t>meme moi je lis pas tout</t>
-  </si>
-  <si>
-    <t>mettre en plus gros les polices</t>
-  </si>
-  <si>
     <t>Checklist #SEO</t>
   </si>
   <si>
-    <t>balise alt sur les images</t>
-  </si>
-  <si>
-    <t>pour savoir ce que représent l'image</t>
-  </si>
-  <si>
-    <t>balises semantiques absentes</t>
-  </si>
-  <si>
     <t>Questions Réponses</t>
   </si>
   <si>
     <t>BootStrap</t>
   </si>
   <si>
-    <t>Checklist #SEO et lighthouse</t>
-  </si>
-  <si>
-    <t>Mettre les balises alt</t>
-  </si>
-  <si>
-    <t>footer ectc en remarques</t>
-  </si>
-  <si>
     <t>OK ?</t>
   </si>
   <si>
@@ -129,15 +87,6 @@
     <t>X</t>
   </si>
   <si>
-    <t>Changement couleur</t>
-  </si>
-  <si>
-    <t>mis du noir daans la footer</t>
-  </si>
-  <si>
-    <t>col-sm4 encadré plus visible</t>
-  </si>
-  <si>
     <t>alt contenait paris</t>
   </si>
   <si>
@@ -147,21 +96,6 @@
     <t>Lien Wave</t>
   </si>
   <si>
-    <t>Je l'ai viré on est a Lyon</t>
-  </si>
-  <si>
-    <t>changé en ombre plus propre</t>
-  </si>
-  <si>
-    <t>label mal placé</t>
-  </si>
-  <si>
-    <t>rajuot du focus</t>
-  </si>
-  <si>
-    <t>rajout du aria label sur icones sociaux</t>
-  </si>
-  <si>
     <t>aria label sur le skiplink</t>
   </si>
   <si>
@@ -379,6 +313,117 @@
   </si>
   <si>
     <t xml:space="preserve">Risque d'etre Blacklisté par Google anciennes pratiques  pas ok </t>
+  </si>
+  <si>
+    <t>Taille de polices  petites sur certaines parties</t>
+  </si>
+  <si>
+    <t>Le Surfeur doit pouvoir acceder facilement a l'information</t>
+  </si>
+  <si>
+    <t>Augment la taille et mettre en gras de temps en temps</t>
+  </si>
+  <si>
+    <t>Penser aux gens mal voyants le faire obligatoirement</t>
+  </si>
+  <si>
+    <t>Pas de Balise alt sur les images</t>
+  </si>
+  <si>
+    <t>Si mauvais connection ou pour les mal voyants on se sait pas ce que c'est</t>
+  </si>
+  <si>
+    <t>Mettre les balises alt et compréhensibles</t>
+  </si>
+  <si>
+    <t>Le Faire et surtout en rapport avec l'image</t>
+  </si>
+  <si>
+    <t>Contraste des couleurs pas assez fort</t>
+  </si>
+  <si>
+    <t>Pour les personnes problemes de vision ( daltoniens ou autres )</t>
+  </si>
+  <si>
+    <t>En parler avec le UI Designer en amont outil pratique a mettre en place</t>
+  </si>
+  <si>
+    <t>Extension Chrome Wave</t>
+  </si>
+  <si>
+    <t>Mettre un fort contraste en respectant la chartre graphique</t>
+  </si>
+  <si>
+    <t>Balises Semantiques absentes</t>
+  </si>
+  <si>
+    <t>Les balises servent autant en SEO qu'en accessibilité</t>
+  </si>
+  <si>
+    <t>Mettre de bonnes balises permet un meilleure lecture</t>
+  </si>
+  <si>
+    <t>Une bonne lecture pour le surfeur et pour le référencement est obligatoire</t>
+  </si>
+  <si>
+    <t>col-sm4 encadré pas très visible</t>
+  </si>
+  <si>
+    <t>Bien séparer les blocks permet une lecture plus simple</t>
+  </si>
+  <si>
+    <t>Mis des ombres pour mieux identifié les blocks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le surfeur peut etre perdu sur ce bloc primordial </t>
+  </si>
+  <si>
+    <t>Pourquoi une balise Alt comprenait Paris alors que l'on est a Lyon ?</t>
+  </si>
+  <si>
+    <t>Mettre des Alt cohérents surtout sur la localisation</t>
+  </si>
+  <si>
+    <t>Certaines personnes écoutent le contenu du site</t>
+  </si>
+  <si>
+    <t>Mettre la langue du site pour meilleure audition</t>
+  </si>
+  <si>
+    <t>Déjà fait dans la partie SEO mais indispensable pour l'accessibilité</t>
+  </si>
+  <si>
+    <t>Dans formulaires les fin de label mal placé</t>
+  </si>
+  <si>
+    <t>Dans le formulaire si les label ne correspondent pas on ne comprends rien</t>
+  </si>
+  <si>
+    <t>Mettre le Label dans le input puis le fermer</t>
+  </si>
+  <si>
+    <t>Les personnes seront enfin quel est le input demandé grace a une meilleure définition</t>
+  </si>
+  <si>
+    <t>Rajout du focus</t>
+  </si>
+  <si>
+    <t>Dans le Formulaire on peut mieux cerner ou on se situe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rajouter un focus </t>
+  </si>
+  <si>
+    <t>Le mettre d'une différentes couleurs ou autres effet</t>
+  </si>
+  <si>
+    <t>Icones des réseaux sociaux mal indiquées</t>
+  </si>
+  <si>
+    <t>Une Balise  aria-label c'est  la balise Alt pour le texte</t>
+  </si>
+  <si>
+    <t>Mettre cette balise ne change rien pour le surf mais permet aux non ou mal voyants de savoir ce que représente le texte</t>
   </si>
 </sst>
 </file>
@@ -445,7 +490,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -458,8 +503,14 @@
         <bgColor rgb="FF7030A0"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFCE4D6"/>
+        <bgColor rgb="FFFCE4D6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -474,12 +525,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFF4B084"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFF4B084"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFF4B084"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -501,6 +565,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1292,16 +1359,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1016"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="40.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="68.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="44.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="55.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="82.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
@@ -1311,7 +1378,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>44</v>
+        <v>22</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -1329,7 +1396,7 @@
         <v>4</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="H1" s="9"/>
       <c r="I1" s="9"/>
@@ -1359,19 +1426,19 @@
         <v>6</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>73</v>
+        <v>51</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -1379,22 +1446,22 @@
         <v>5</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>54</v>
+        <v>32</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>53</v>
+        <v>31</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -1402,22 +1469,22 @@
         <v>5</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>49</v>
+        <v>27</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>57</v>
+        <v>35</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -1425,22 +1492,22 @@
         <v>5</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>51</v>
+        <v>29</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>52</v>
+        <v>30</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -1448,22 +1515,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>15</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="G6" s="4" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -1471,22 +1538,22 @@
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>62</v>
+        <v>40</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -1494,22 +1561,22 @@
         <v>5</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>64</v>
+        <v>42</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>65</v>
+        <v>43</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -1517,22 +1584,22 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>67</v>
+        <v>45</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -1540,20 +1607,20 @@
         <v>5</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>74</v>
+        <v>52</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>75</v>
+        <v>53</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>76</v>
+        <v>54</v>
       </c>
       <c r="E10" s="10"/>
       <c r="F10" s="11" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -1561,20 +1628,20 @@
         <v>5</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>77</v>
+        <v>55</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>79</v>
+        <v>57</v>
       </c>
       <c r="E11" s="10"/>
       <c r="F11" s="11" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -1582,22 +1649,22 @@
         <v>5</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>81</v>
+        <v>59</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>82</v>
+        <v>60</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>83</v>
+        <v>61</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -1605,20 +1672,20 @@
         <v>5</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>84</v>
+        <v>62</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="10" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -1626,22 +1693,22 @@
         <v>5</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>86</v>
+        <v>64</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>87</v>
+        <v>65</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>89</v>
+        <v>67</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -1649,22 +1716,22 @@
         <v>5</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>91</v>
+        <v>69</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -1672,22 +1739,22 @@
         <v>5</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>96</v>
+        <v>74</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -1695,22 +1762,22 @@
         <v>5</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>94</v>
+        <v>72</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>97</v>
+        <v>75</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -1718,22 +1785,22 @@
         <v>5</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>99</v>
+        <v>77</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>100</v>
+        <v>78</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>101</v>
+        <v>79</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -1741,22 +1808,22 @@
         <v>5</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>102</v>
+        <v>80</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>103</v>
+        <v>81</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>88</v>
+        <v>66</v>
       </c>
       <c r="E19" s="10" t="s">
-        <v>85</v>
+        <v>63</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -1764,22 +1831,22 @@
         <v>5</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>30</v>
+        <v>16</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>104</v>
+        <v>82</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>105</v>
+        <v>83</v>
       </c>
       <c r="E20" s="10" t="s">
-        <v>106</v>
+        <v>84</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="G20" s="4" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -1787,22 +1854,22 @@
         <v>5</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>108</v>
+        <v>86</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>109</v>
+        <v>87</v>
       </c>
       <c r="E21" s="10" t="s">
-        <v>110</v>
+        <v>88</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>92</v>
+        <v>70</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -1810,22 +1877,22 @@
         <v>5</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>111</v>
+        <v>89</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>112</v>
+        <v>90</v>
       </c>
       <c r="E22" s="10" t="s">
-        <v>113</v>
+        <v>91</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="G22" s="12" t="s">
-        <v>31</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
@@ -1839,178 +1906,234 @@
     </row>
     <row r="24" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>16</v>
+        <v>94</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>17</v>
+        <v>95</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>18</v>
+        <v>96</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G24" s="4"/>
+        <v>97</v>
+      </c>
+      <c r="F24" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="25" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>20</v>
+        <v>98</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>21</v>
+        <v>99</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>26</v>
+        <v>100</v>
       </c>
       <c r="E25" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G25" s="4"/>
+        <v>101</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="26" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>32</v>
+        <v>102</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
+        <v>103</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="27" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>22</v>
+        <v>107</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>27</v>
+        <v>108</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>14</v>
+        <v>109</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>14</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G27" s="4"/>
+        <v>110</v>
+      </c>
+      <c r="F27" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="28" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>34</v>
+        <v>111</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
+        <v>114</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="E28" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="29" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>35</v>
+        <v>18</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D29" s="5"/>
-      <c r="E29" s="5"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
+        <v>115</v>
+      </c>
+      <c r="D29" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="E29" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="F29" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="30" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>9</v>
+        <v>117</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>10</v>
+        <v>118</v>
       </c>
       <c r="E30" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G30" s="4"/>
+        <v>119</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="31" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="10"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
+        <v>120</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="32" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
+        <v>124</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="33" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
+        <v>128</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>130</v>
+      </c>
       <c r="E33" s="5"/>
       <c r="F33" s="4"/>
       <c r="G33" s="4"/>
     </row>
     <row r="34" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>43</v>
+        <v>21</v>
       </c>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
@@ -2031,10 +2154,10 @@
       <c r="A36" s="5"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5" t="s">
-        <v>36</v>
+        <v>19</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>37</v>
+        <v>20</v>
       </c>
       <c r="E36" s="5"/>
       <c r="F36" s="4"/>
@@ -3043,12 +3166,21 @@
     <hyperlink ref="F20" r:id="rId19" xr:uid="{9940974C-2DE6-C849-8FFF-E00D77703634}"/>
     <hyperlink ref="F21" r:id="rId20" xr:uid="{1ECF8826-8E64-8C4D-A5C5-F3A4B120FC8A}"/>
     <hyperlink ref="F22" r:id="rId21" xr:uid="{CCDE431B-14C3-8D46-8EAB-D188D8E8C8A5}"/>
+    <hyperlink ref="F24" r:id="rId22" xr:uid="{97697197-9AC2-DD4E-B736-F41F18C35D48}"/>
+    <hyperlink ref="F25" r:id="rId23" xr:uid="{1539DEE0-BB06-DB47-AF1C-6B209EF12EA0}"/>
+    <hyperlink ref="F26" r:id="rId24" xr:uid="{599ACF77-59D0-D14B-BE6E-6D952E5B07E0}"/>
+    <hyperlink ref="F27" r:id="rId25" xr:uid="{ED097B17-7FB9-9545-80E2-0E98276AA57C}"/>
+    <hyperlink ref="F28" r:id="rId26" xr:uid="{F00B7C1F-69A4-D940-BB2A-1A193C945363}"/>
+    <hyperlink ref="F29" r:id="rId27" xr:uid="{08D195A8-7329-AF49-8E35-335DF52BC222}"/>
+    <hyperlink ref="F30" r:id="rId28" xr:uid="{DA68F960-859B-194D-9CB5-2AB7FFB6A949}"/>
+    <hyperlink ref="F31" r:id="rId29" xr:uid="{76D83CA0-53C9-4B4F-A51A-49D6B94E80E3}"/>
+    <hyperlink ref="F32" r:id="rId30" xr:uid="{56FC4D89-7BAB-FC4C-8DDC-EC85DFE97FA8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId22"/>
+  <drawing r:id="rId31"/>
   <tableParts count="1">
-    <tablePart r:id="rId23"/>
+    <tablePart r:id="rId32"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Site 100% Tableau 100% Now PowerPoint
Maintenant le PowerPoint
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fred/Desktop/OpenClassRoom/P4 Vrac/ProjetP4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{077AEFDB-1CB6-1B45-99E6-540ACFB39F9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3661C2-D56F-F842-B887-35BA16E39278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3100" yWindow="4780" windowWidth="46880" windowHeight="19880" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1920" yWindow="1160" windowWidth="46580" windowHeight="24620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="132">
   <si>
     <t>Problème identifié</t>
   </si>
@@ -90,15 +90,6 @@
     <t>alt contenait paris</t>
   </si>
   <si>
-    <t>installer l'extension chrome wave</t>
-  </si>
-  <si>
-    <t>Lien Wave</t>
-  </si>
-  <si>
-    <t>aria label sur le skiplink</t>
-  </si>
-  <si>
     <t>CAT</t>
   </si>
   <si>
@@ -424,6 +415,18 @@
   </si>
   <si>
     <t>Mettre cette balise ne change rien pour le surf mais permet aux non ou mal voyants de savoir ce que représente le texte</t>
+  </si>
+  <si>
+    <t>Certaines personnes se déplace dans les zones grace a la tabulation</t>
+  </si>
+  <si>
+    <t>Mettre un Skiplink permet de surfer grace au clavier</t>
+  </si>
+  <si>
+    <t>En rajoutant un aria label sur le skiplink permet de ne pas changer le site</t>
+  </si>
+  <si>
+    <t>Le formulaire pas accessible</t>
   </si>
 </sst>
 </file>
@@ -543,7 +546,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -558,7 +561,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
@@ -712,440 +714,9 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:oneCellAnchor>
-    <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>4603750</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
-    </xdr:from>
-    <xdr:ext cx="4464050" cy="749300"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
-      <mc:Choice Requires="a14">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2" name="ZoneTexte 1">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE973A8B-D8E7-CE4D-8CF9-D47EF54E146E}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="18256250" y="5969000"/>
-              <a:ext cx="4464050" cy="749300"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:noAutofit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a14:m>
-                <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                  <m:oMathParaPr>
-                    <m:jc m:val="centerGroup"/>
-                  </m:oMathParaPr>
-                  <m:oMath xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
-                    <m:r>
-                      <a:rPr lang="fr-FR" sz="1100" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>𝑓</m:t>
-                    </m:r>
-                    <m:d>
-                      <m:dPr>
-                        <m:ctrlPr>
-                          <a:rPr lang="fr-FR" sz="1100" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                        </m:ctrlPr>
-                      </m:dPr>
-                      <m:e>
-                        <m:r>
-                          <a:rPr lang="fr-FR" sz="1100" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑥</m:t>
-                        </m:r>
-                      </m:e>
-                    </m:d>
-                    <m:r>
-                      <a:rPr lang="fr-FR" sz="1100" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>=</m:t>
-                    </m:r>
-                    <m:sSub>
-                      <m:sSubPr>
-                        <m:ctrlPr>
-                          <a:rPr lang="fr-FR" sz="1100" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                        </m:ctrlPr>
-                      </m:sSubPr>
-                      <m:e>
-                        <m:r>
-                          <a:rPr lang="fr-FR" sz="1100" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑎</m:t>
-                        </m:r>
-                      </m:e>
-                      <m:sub>
-                        <m:r>
-                          <a:rPr lang="fr-FR" sz="1100" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>0</m:t>
-                        </m:r>
-                      </m:sub>
-                    </m:sSub>
-                    <m:r>
-                      <a:rPr lang="fr-FR" sz="1100" i="1">
-                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                      </a:rPr>
-                      <m:t>+</m:t>
-                    </m:r>
-                    <m:nary>
-                      <m:naryPr>
-                        <m:chr m:val="∑"/>
-                        <m:ctrlPr>
-                          <a:rPr lang="fr-FR" sz="1100" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                        </m:ctrlPr>
-                      </m:naryPr>
-                      <m:sub>
-                        <m:r>
-                          <a:rPr lang="fr-FR" sz="1100" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>𝑛</m:t>
-                        </m:r>
-                        <m:r>
-                          <a:rPr lang="fr-FR" sz="1100" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>=1</m:t>
-                        </m:r>
-                      </m:sub>
-                      <m:sup>
-                        <m:r>
-                          <a:rPr lang="fr-FR" sz="1100" i="1">
-                            <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                          </a:rPr>
-                          <m:t>∞</m:t>
-                        </m:r>
-                      </m:sup>
-                      <m:e>
-                        <m:d>
-                          <m:dPr>
-                            <m:ctrlPr>
-                              <a:rPr lang="fr-FR" sz="1100" i="1">
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              </a:rPr>
-                            </m:ctrlPr>
-                          </m:dPr>
-                          <m:e>
-                            <m:sSub>
-                              <m:sSubPr>
-                                <m:ctrlPr>
-                                  <a:rPr lang="fr-FR" sz="1100" i="1">
-                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                  </a:rPr>
-                                </m:ctrlPr>
-                              </m:sSubPr>
-                              <m:e>
-                                <m:r>
-                                  <a:rPr lang="fr-FR" sz="1100" i="1">
-                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                  </a:rPr>
-                                  <m:t>𝑎</m:t>
-                                </m:r>
-                              </m:e>
-                              <m:sub>
-                                <m:r>
-                                  <a:rPr lang="fr-FR" sz="1100" i="1">
-                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                  </a:rPr>
-                                  <m:t>𝑛</m:t>
-                                </m:r>
-                              </m:sub>
-                            </m:sSub>
-                            <m:func>
-                              <m:funcPr>
-                                <m:ctrlPr>
-                                  <a:rPr lang="fr-FR" sz="1100" i="1">
-                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                  </a:rPr>
-                                </m:ctrlPr>
-                              </m:funcPr>
-                              <m:fName>
-                                <m:r>
-                                  <m:rPr>
-                                    <m:sty m:val="p"/>
-                                  </m:rPr>
-                                  <a:rPr lang="fr-FR" sz="1100" i="0">
-                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                  </a:rPr>
-                                  <m:t>cos</m:t>
-                                </m:r>
-                              </m:fName>
-                              <m:e>
-                                <m:f>
-                                  <m:fPr>
-                                    <m:ctrlPr>
-                                      <a:rPr lang="fr-FR" sz="1100" i="1">
-                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                      </a:rPr>
-                                    </m:ctrlPr>
-                                  </m:fPr>
-                                  <m:num>
-                                    <m:r>
-                                      <a:rPr lang="fr-FR" sz="1100" i="1">
-                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                      </a:rPr>
-                                      <m:t>𝑛</m:t>
-                                    </m:r>
-                                    <m:r>
-                                      <a:rPr lang="el-GR" sz="1100" i="1">
-                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                      </a:rPr>
-                                      <m:t>𝜋</m:t>
-                                    </m:r>
-                                    <m:r>
-                                      <a:rPr lang="fr-FR" sz="1100" i="1">
-                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                      </a:rPr>
-                                      <m:t>𝑥</m:t>
-                                    </m:r>
-                                  </m:num>
-                                  <m:den>
-                                    <m:r>
-                                      <a:rPr lang="fr-FR" sz="1100" i="1">
-                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                      </a:rPr>
-                                      <m:t>𝐿</m:t>
-                                    </m:r>
-                                  </m:den>
-                                </m:f>
-                              </m:e>
-                            </m:func>
-                            <m:r>
-                              <a:rPr lang="fr-FR" sz="1100" i="1">
-                                <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                              </a:rPr>
-                              <m:t>+</m:t>
-                            </m:r>
-                            <m:sSub>
-                              <m:sSubPr>
-                                <m:ctrlPr>
-                                  <a:rPr lang="fr-FR" sz="1100" i="1">
-                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                  </a:rPr>
-                                </m:ctrlPr>
-                              </m:sSubPr>
-                              <m:e>
-                                <m:r>
-                                  <a:rPr lang="fr-FR" sz="1100" i="1">
-                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                  </a:rPr>
-                                  <m:t>𝑏</m:t>
-                                </m:r>
-                              </m:e>
-                              <m:sub>
-                                <m:r>
-                                  <a:rPr lang="fr-FR" sz="1100" i="1">
-                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                  </a:rPr>
-                                  <m:t>𝑛</m:t>
-                                </m:r>
-                              </m:sub>
-                            </m:sSub>
-                            <m:func>
-                              <m:funcPr>
-                                <m:ctrlPr>
-                                  <a:rPr lang="fr-FR" sz="1100" i="1">
-                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                  </a:rPr>
-                                </m:ctrlPr>
-                              </m:funcPr>
-                              <m:fName>
-                                <m:r>
-                                  <m:rPr>
-                                    <m:sty m:val="p"/>
-                                  </m:rPr>
-                                  <a:rPr lang="fr-FR" sz="1100" i="0">
-                                    <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                  </a:rPr>
-                                  <m:t>sin</m:t>
-                                </m:r>
-                              </m:fName>
-                              <m:e>
-                                <m:f>
-                                  <m:fPr>
-                                    <m:ctrlPr>
-                                      <a:rPr lang="fr-FR" sz="1100" i="1">
-                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                      </a:rPr>
-                                    </m:ctrlPr>
-                                  </m:fPr>
-                                  <m:num>
-                                    <m:r>
-                                      <a:rPr lang="fr-FR" sz="1100" i="1">
-                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                      </a:rPr>
-                                      <m:t>𝑛</m:t>
-                                    </m:r>
-                                    <m:r>
-                                      <a:rPr lang="el-GR" sz="1100" i="1">
-                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                      </a:rPr>
-                                      <m:t>𝜋</m:t>
-                                    </m:r>
-                                    <m:r>
-                                      <a:rPr lang="fr-FR" sz="1100" i="1">
-                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                      </a:rPr>
-                                      <m:t>𝑥</m:t>
-                                    </m:r>
-                                  </m:num>
-                                  <m:den>
-                                    <m:r>
-                                      <a:rPr lang="fr-FR" sz="1100" i="1">
-                                        <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                                      </a:rPr>
-                                      <m:t>𝐿</m:t>
-                                    </m:r>
-                                  </m:den>
-                                </m:f>
-                              </m:e>
-                            </m:func>
-                          </m:e>
-                        </m:d>
-                      </m:e>
-                    </m:nary>
-                  </m:oMath>
-                </m:oMathPara>
-              </a14:m>
-              <a:endParaRPr lang="fr-FR" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Choice>
-      <mc:Fallback xmlns="">
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="2" name="ZoneTexte 1">
-              <a:extLst>
-                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BE973A8B-D8E7-CE4D-8CF9-D47EF54E146E}"/>
-                </a:ext>
-              </a:extLst>
-            </xdr:cNvPr>
-            <xdr:cNvSpPr txBox="1"/>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:xfrm>
-              <a:off x="18256250" y="5969000"/>
-              <a:ext cx="4464050" cy="749300"/>
-            </a:xfrm>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:noFill/>
-          </xdr:spPr>
-          <xdr:style>
-            <a:lnRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:lnRef>
-            <a:fillRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:fillRef>
-            <a:effectRef idx="0">
-              <a:scrgbClr r="0" g="0" b="0"/>
-            </a:effectRef>
-            <a:fontRef idx="minor">
-              <a:schemeClr val="tx1"/>
-            </a:fontRef>
-          </xdr:style>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
-              <a:noAutofit/>
-            </a:bodyPr>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr/>
-              <a:r>
-                <a:rPr lang="fr-FR" sz="1100" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>𝑓(𝑥)=𝑎_0+∑_(𝑛=1)^∞▒(𝑎_𝑛  cos⁡〖𝑛</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="el-GR" sz="1100" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>𝜋</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="fr-FR" sz="1100" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>𝑥/𝐿〗+𝑏_𝑛  sin⁡〖𝑛</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="el-GR" sz="1100" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>𝜋</a:t>
-              </a:r>
-              <a:r>
-                <a:rPr lang="fr-FR" sz="1100" i="0">
-                  <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
-                </a:rPr>
-                <a:t>𝑥/𝐿〗 ) </a:t>
-              </a:r>
-              <a:endParaRPr lang="fr-FR" sz="1100"/>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:oneCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E796EE32-1DFE-CD45-A2AF-F728FFC58B5F}" name="Tableau1" displayName="Tableau1" ref="A1:G36" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:G36" xr:uid="{E796EE32-1DFE-CD45-A2AF-F728FFC58B5F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E796EE32-1DFE-CD45-A2AF-F728FFC58B5F}" name="Tableau1" displayName="Tableau1" ref="A1:G34" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:G34" xr:uid="{E796EE32-1DFE-CD45-A2AF-F728FFC58B5F}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{9BB85078-D1DA-EA4F-939E-EA2B94AC6A91}" name="CAT" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{701895DD-CBC8-C945-8BB8-1AF30E309D3E}" name="Problème identifié" dataDxfId="7"/>
@@ -1357,10 +928,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1016"/>
+  <dimension ref="A1:Z1014"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1378,7 +949,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>0</v>
@@ -1398,25 +969,25 @@
       <c r="G1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="9"/>
-      <c r="X1" s="9"/>
-      <c r="Y1" s="9"/>
-      <c r="Z1" s="9"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8"/>
     </row>
     <row r="2" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
@@ -1426,16 +997,16 @@
         <v>6</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="E2" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="F2" s="11" t="s">
-        <v>36</v>
+        <v>47</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>15</v>
@@ -1446,19 +1017,19 @@
         <v>5</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="F3" s="10" t="s">
         <v>33</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="F3" s="11" t="s">
-        <v>36</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>15</v>
@@ -1472,16 +1043,16 @@
         <v>7</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="E4" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" s="11" t="s">
-        <v>36</v>
+      <c r="E4" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>15</v>
@@ -1495,16 +1066,16 @@
         <v>9</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="11" t="s">
-        <v>36</v>
+        <v>26</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>15</v>
@@ -1518,16 +1089,16 @@
         <v>10</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="E6" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="11" t="s">
-        <v>36</v>
+        <v>23</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>15</v>
@@ -1538,19 +1109,19 @@
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C7" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="F7" s="11" t="s">
-        <v>36</v>
+      <c r="F7" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>15</v>
@@ -1561,19 +1132,19 @@
         <v>5</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="F8" s="10" t="s">
         <v>42</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="F8" s="11" t="s">
-        <v>45</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>15</v>
@@ -1584,19 +1155,19 @@
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="F9" s="11" t="s">
         <v>45</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>42</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>15</v>
@@ -1607,17 +1178,17 @@
         <v>5</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="E10" s="10"/>
-      <c r="F10" s="11" t="s">
-        <v>36</v>
+        <v>51</v>
+      </c>
+      <c r="E10" s="9"/>
+      <c r="F10" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>15</v>
@@ -1628,17 +1199,17 @@
         <v>5</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="E11" s="10"/>
-      <c r="F11" s="11" t="s">
-        <v>36</v>
+        <v>54</v>
+      </c>
+      <c r="E11" s="9"/>
+      <c r="F11" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>15</v>
@@ -1649,19 +1220,19 @@
         <v>5</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="E12" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="C12" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="E12" s="10" t="s">
-        <v>61</v>
-      </c>
-      <c r="F12" s="11" t="s">
-        <v>36</v>
+      <c r="F12" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>15</v>
@@ -1672,19 +1243,19 @@
         <v>5</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="D13" s="5"/>
-      <c r="E13" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="F13" s="11" t="s">
+      <c r="E13" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="F13" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="G13" s="11" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1693,21 +1264,21 @@
         <v>5</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="E14" s="10" t="s">
+      <c r="F14" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="F14" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="G14" s="12" t="s">
+      <c r="G14" s="11" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1719,18 +1290,18 @@
         <v>12</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="F15" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="F15" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G15" s="12" t="s">
+      <c r="G15" s="11" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1742,18 +1313,18 @@
         <v>13</v>
       </c>
       <c r="C16" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="F16" s="10" t="s">
         <v>72</v>
       </c>
-      <c r="D16" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>75</v>
-      </c>
-      <c r="G16" s="12" t="s">
+      <c r="G16" s="11" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1762,19 +1333,19 @@
         <v>5</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C17" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="F17" s="10" t="s">
         <v>72</v>
-      </c>
-      <c r="D17" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>76</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>75</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>15</v>
@@ -1785,18 +1356,18 @@
         <v>5</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="F18" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="F18" s="10" t="s">
         <v>11</v>
       </c>
       <c r="G18" s="4" t="s">
@@ -1808,21 +1379,21 @@
         <v>5</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="E19" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="F19" s="11" t="s">
+      <c r="E19" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="F19" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G19" s="12" t="s">
+      <c r="G19" s="11" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1834,16 +1405,16 @@
         <v>16</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>84</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>36</v>
+        <v>80</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>15</v>
@@ -1854,19 +1425,19 @@
         <v>5</v>
       </c>
       <c r="B21" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E21" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="C21" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="D21" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>88</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>70</v>
+      <c r="F21" s="10" t="s">
+        <v>67</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>15</v>
@@ -1877,21 +1448,21 @@
         <v>5</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="F22" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="E22" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="F22" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="G22" s="12" t="s">
+      <c r="G22" s="11" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1900,28 +1471,28 @@
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
-      <c r="E23" s="10"/>
+      <c r="E23" s="9"/>
       <c r="F23" s="4"/>
       <c r="G23" s="4"/>
     </row>
     <row r="24" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B24" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="E24" s="9" t="s">
         <v>94</v>
       </c>
-      <c r="C24" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="D24" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>36</v>
+      <c r="F24" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>15</v>
@@ -1929,22 +1500,22 @@
     </row>
     <row r="25" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B25" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D25" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="E25" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="C25" s="5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D25" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>75</v>
+      <c r="F25" s="10" t="s">
+        <v>72</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>15</v>
@@ -1952,22 +1523,22 @@
     </row>
     <row r="26" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B26" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="E26" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="F26" s="12" t="s">
         <v>102</v>
-      </c>
-      <c r="C26" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="D26" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="F26" s="13" t="s">
-        <v>105</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>15</v>
@@ -1975,22 +1546,22 @@
     </row>
     <row r="27" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B27" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C27" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D27" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="E27" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="C27" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="E27" s="10" t="s">
-        <v>110</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>75</v>
+      <c r="F27" s="10" t="s">
+        <v>72</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>15</v>
@@ -1998,22 +1569,22 @@
     </row>
     <row r="28" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B28" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C28" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="C28" s="5" t="s">
-        <v>114</v>
-      </c>
       <c r="D28" s="5" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="F28" s="11" t="s">
-        <v>70</v>
+        <v>110</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>67</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>15</v>
@@ -2021,22 +1592,22 @@
     </row>
     <row r="29" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B29" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>116</v>
-      </c>
-      <c r="E29" s="10" t="s">
-        <v>97</v>
-      </c>
-      <c r="F29" s="11" t="s">
-        <v>36</v>
+        <v>113</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>15</v>
@@ -2044,22 +1615,22 @@
     </row>
     <row r="30" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="F30" s="11" t="s">
-        <v>36</v>
+        <v>115</v>
+      </c>
+      <c r="E30" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>33</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>15</v>
@@ -2067,22 +1638,22 @@
     </row>
     <row r="31" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B31" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="D31" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E31" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="C31" s="5" t="s">
-        <v>121</v>
-      </c>
-      <c r="D31" s="5" t="s">
-        <v>122</v>
-      </c>
-      <c r="E31" s="10" t="s">
-        <v>123</v>
-      </c>
-      <c r="F31" s="11" t="s">
-        <v>75</v>
+      <c r="F31" s="10" t="s">
+        <v>72</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>15</v>
@@ -2090,22 +1661,22 @@
     </row>
     <row r="32" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B32" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>122</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="E32" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="C32" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="D32" s="5" t="s">
-        <v>126</v>
-      </c>
-      <c r="E32" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="F32" s="11" t="s">
-        <v>75</v>
+      <c r="F32" s="10" t="s">
+        <v>72</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>15</v>
@@ -2113,56 +1684,50 @@
     </row>
     <row r="33" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="E33" s="5"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
+      <c r="F33" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="34" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
-      <c r="E34" s="5"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-    </row>
-    <row r="35" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="5"/>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
-    </row>
-    <row r="36" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="5"/>
-      <c r="B36" s="5"/>
-      <c r="C36" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="E36" s="5"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-    </row>
+        <v>131</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="E34" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -3141,44 +2706,42 @@
     <row r="1012" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1013" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1014" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1015" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1016" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C10" r:id="rId1" display="https://fredericguilet.github.io/P4Guillet_Frederic25072021/voiture.com" xr:uid="{F0E0A3CD-37FD-9E44-B979-49DC1760F2BE}"/>
     <hyperlink ref="C11" r:id="rId2" display="https://fredericguilet.github.io/P4Guillet_Frederic25072021/pizza.com" xr:uid="{68CF73CC-7EFC-0048-B22E-4CE39E7A4D9F}"/>
-    <hyperlink ref="D36" r:id="rId3" xr:uid="{8B9623D5-26B1-F54A-9395-E5EC71494DBA}"/>
-    <hyperlink ref="F2" r:id="rId4" xr:uid="{DF56BA83-E4D7-3D49-8E46-5DA1D7F0BF6B}"/>
-    <hyperlink ref="F3:F6" r:id="rId5" display="OpenClassRooms" xr:uid="{FBEF5557-F283-B44B-8AD5-18C42F6301B5}"/>
-    <hyperlink ref="F7" r:id="rId6" xr:uid="{210A7551-794E-B34C-AA75-9FCA644AE40B}"/>
-    <hyperlink ref="F8" r:id="rId7" xr:uid="{140B208B-D31E-214A-A1BB-CDC3896E4F8F}"/>
-    <hyperlink ref="F9" r:id="rId8" xr:uid="{1CAF9DA3-EF35-E54A-87AB-439617F277AE}"/>
-    <hyperlink ref="F10" r:id="rId9" xr:uid="{ECC056D8-7AF8-064A-B011-2942CAFE8449}"/>
-    <hyperlink ref="F11" r:id="rId10" xr:uid="{9841D446-7B53-634A-883A-63FC63860DF9}"/>
-    <hyperlink ref="F12" r:id="rId11" xr:uid="{FFA3C916-33BF-324A-B768-5845F53E3B1C}"/>
-    <hyperlink ref="F13" r:id="rId12" xr:uid="{B1BAF8CE-606D-0B4F-8428-237F8CD57312}"/>
-    <hyperlink ref="F14" r:id="rId13" xr:uid="{2BFE7964-3028-644D-945B-22C79D77C8CC}"/>
-    <hyperlink ref="F15" r:id="rId14" xr:uid="{9BB76B05-4769-6A4A-BFE9-AB49E1089187}"/>
-    <hyperlink ref="F16" r:id="rId15" xr:uid="{E6818DFB-78F2-D143-A048-0EDCA090BB9A}"/>
-    <hyperlink ref="F17" r:id="rId16" xr:uid="{BCB0B4D9-E802-A641-8202-DEF07D85A9DE}"/>
-    <hyperlink ref="F18" r:id="rId17" xr:uid="{D21035A4-8923-904D-AB29-B185D2CBCBA9}"/>
-    <hyperlink ref="F19" r:id="rId18" xr:uid="{9B5ED51E-C284-A849-8F3A-BB456B5C58A6}"/>
-    <hyperlink ref="F20" r:id="rId19" xr:uid="{9940974C-2DE6-C849-8FFF-E00D77703634}"/>
-    <hyperlink ref="F21" r:id="rId20" xr:uid="{1ECF8826-8E64-8C4D-A5C5-F3A4B120FC8A}"/>
-    <hyperlink ref="F22" r:id="rId21" xr:uid="{CCDE431B-14C3-8D46-8EAB-D188D8E8C8A5}"/>
-    <hyperlink ref="F24" r:id="rId22" xr:uid="{97697197-9AC2-DD4E-B736-F41F18C35D48}"/>
-    <hyperlink ref="F25" r:id="rId23" xr:uid="{1539DEE0-BB06-DB47-AF1C-6B209EF12EA0}"/>
-    <hyperlink ref="F26" r:id="rId24" xr:uid="{599ACF77-59D0-D14B-BE6E-6D952E5B07E0}"/>
-    <hyperlink ref="F27" r:id="rId25" xr:uid="{ED097B17-7FB9-9545-80E2-0E98276AA57C}"/>
-    <hyperlink ref="F28" r:id="rId26" xr:uid="{F00B7C1F-69A4-D940-BB2A-1A193C945363}"/>
-    <hyperlink ref="F29" r:id="rId27" xr:uid="{08D195A8-7329-AF49-8E35-335DF52BC222}"/>
-    <hyperlink ref="F30" r:id="rId28" xr:uid="{DA68F960-859B-194D-9CB5-2AB7FFB6A949}"/>
-    <hyperlink ref="F31" r:id="rId29" xr:uid="{76D83CA0-53C9-4B4F-A51A-49D6B94E80E3}"/>
-    <hyperlink ref="F32" r:id="rId30" xr:uid="{56FC4D89-7BAB-FC4C-8DDC-EC85DFE97FA8}"/>
+    <hyperlink ref="F2" r:id="rId3" xr:uid="{DF56BA83-E4D7-3D49-8E46-5DA1D7F0BF6B}"/>
+    <hyperlink ref="F3:F6" r:id="rId4" display="OpenClassRooms" xr:uid="{FBEF5557-F283-B44B-8AD5-18C42F6301B5}"/>
+    <hyperlink ref="F7" r:id="rId5" xr:uid="{210A7551-794E-B34C-AA75-9FCA644AE40B}"/>
+    <hyperlink ref="F8" r:id="rId6" xr:uid="{140B208B-D31E-214A-A1BB-CDC3896E4F8F}"/>
+    <hyperlink ref="F9" r:id="rId7" xr:uid="{1CAF9DA3-EF35-E54A-87AB-439617F277AE}"/>
+    <hyperlink ref="F10" r:id="rId8" xr:uid="{ECC056D8-7AF8-064A-B011-2942CAFE8449}"/>
+    <hyperlink ref="F11" r:id="rId9" xr:uid="{9841D446-7B53-634A-883A-63FC63860DF9}"/>
+    <hyperlink ref="F12" r:id="rId10" xr:uid="{FFA3C916-33BF-324A-B768-5845F53E3B1C}"/>
+    <hyperlink ref="F13" r:id="rId11" xr:uid="{B1BAF8CE-606D-0B4F-8428-237F8CD57312}"/>
+    <hyperlink ref="F14" r:id="rId12" xr:uid="{2BFE7964-3028-644D-945B-22C79D77C8CC}"/>
+    <hyperlink ref="F15" r:id="rId13" xr:uid="{9BB76B05-4769-6A4A-BFE9-AB49E1089187}"/>
+    <hyperlink ref="F16" r:id="rId14" xr:uid="{E6818DFB-78F2-D143-A048-0EDCA090BB9A}"/>
+    <hyperlink ref="F17" r:id="rId15" xr:uid="{BCB0B4D9-E802-A641-8202-DEF07D85A9DE}"/>
+    <hyperlink ref="F18" r:id="rId16" xr:uid="{D21035A4-8923-904D-AB29-B185D2CBCBA9}"/>
+    <hyperlink ref="F19" r:id="rId17" xr:uid="{9B5ED51E-C284-A849-8F3A-BB456B5C58A6}"/>
+    <hyperlink ref="F20" r:id="rId18" xr:uid="{9940974C-2DE6-C849-8FFF-E00D77703634}"/>
+    <hyperlink ref="F21" r:id="rId19" xr:uid="{1ECF8826-8E64-8C4D-A5C5-F3A4B120FC8A}"/>
+    <hyperlink ref="F22" r:id="rId20" xr:uid="{CCDE431B-14C3-8D46-8EAB-D188D8E8C8A5}"/>
+    <hyperlink ref="F24" r:id="rId21" xr:uid="{97697197-9AC2-DD4E-B736-F41F18C35D48}"/>
+    <hyperlink ref="F25" r:id="rId22" xr:uid="{1539DEE0-BB06-DB47-AF1C-6B209EF12EA0}"/>
+    <hyperlink ref="F26" r:id="rId23" xr:uid="{599ACF77-59D0-D14B-BE6E-6D952E5B07E0}"/>
+    <hyperlink ref="F27" r:id="rId24" xr:uid="{ED097B17-7FB9-9545-80E2-0E98276AA57C}"/>
+    <hyperlink ref="F28" r:id="rId25" xr:uid="{F00B7C1F-69A4-D940-BB2A-1A193C945363}"/>
+    <hyperlink ref="F29" r:id="rId26" xr:uid="{08D195A8-7329-AF49-8E35-335DF52BC222}"/>
+    <hyperlink ref="F30" r:id="rId27" xr:uid="{DA68F960-859B-194D-9CB5-2AB7FFB6A949}"/>
+    <hyperlink ref="F31" r:id="rId28" xr:uid="{76D83CA0-53C9-4B4F-A51A-49D6B94E80E3}"/>
+    <hyperlink ref="F32" r:id="rId29" xr:uid="{56FC4D89-7BAB-FC4C-8DDC-EC85DFE97FA8}"/>
+    <hyperlink ref="F33" r:id="rId30" xr:uid="{4DCD383E-1603-114E-83C8-FC52DEC40B13}"/>
+    <hyperlink ref="F34" r:id="rId31" xr:uid="{5BE6480B-CCB2-8044-87D5-FB762BC0C983}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
-  <drawing r:id="rId31"/>
   <tableParts count="1">
     <tablePart r:id="rId32"/>
   </tableParts>

</xml_diff>

<commit_message>
Grrr Le W3C erreur
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fred/Desktop/OpenClassRoom/P4 Vrac/ProjetP4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB3661C2-D56F-F842-B887-35BA16E39278}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9A75649-79B8-0F49-82BF-6D185CCE5391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="1160" windowWidth="46580" windowHeight="24620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="136">
   <si>
     <t>Problème identifié</t>
   </si>
@@ -427,6 +427,18 @@
   </si>
   <si>
     <t>Le formulaire pas accessible</t>
+  </si>
+  <si>
+    <t>Correction sur le W3CC en CSS</t>
+  </si>
+  <si>
+    <t>plein d'erreur bootstrap</t>
+  </si>
+  <si>
+    <t>Correction sur le W3CC en html</t>
+  </si>
+  <si>
+    <t>Erreur a regarder</t>
   </si>
 </sst>
 </file>
@@ -630,31 +642,6 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color rgb="FFFFFFFF"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF7030A0"/>
-          <bgColor rgb="FF7030A0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <strike val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
@@ -701,6 +688,31 @@
         <scheme val="none"/>
       </font>
     </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color rgb="FFFFFFFF"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF7030A0"/>
+          <bgColor rgb="FF7030A0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
@@ -715,16 +727,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E796EE32-1DFE-CD45-A2AF-F728FFC58B5F}" name="Tableau1" displayName="Tableau1" ref="A1:G34" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E796EE32-1DFE-CD45-A2AF-F728FFC58B5F}" name="Tableau1" displayName="Tableau1" ref="A1:G34" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A1:G34" xr:uid="{E796EE32-1DFE-CD45-A2AF-F728FFC58B5F}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{9BB85078-D1DA-EA4F-939E-EA2B94AC6A91}" name="CAT" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{701895DD-CBC8-C945-8BB8-1AF30E309D3E}" name="Problème identifié" dataDxfId="7"/>
-    <tableColumn id="3" xr3:uid="{8B278B00-9A53-D541-81DA-33000B0C5DCC}" name="Explication du problème" dataDxfId="6"/>
-    <tableColumn id="4" xr3:uid="{4C6455B9-1BC5-7D47-B3D3-56985A6D57BE}" name="Bonne pratique à adopter" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{9BB85078-D1DA-EA4F-939E-EA2B94AC6A91}" name="CAT" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{701895DD-CBC8-C945-8BB8-1AF30E309D3E}" name="Problème identifié" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{8B278B00-9A53-D541-81DA-33000B0C5DCC}" name="Explication du problème" dataDxfId="4"/>
+    <tableColumn id="4" xr3:uid="{4C6455B9-1BC5-7D47-B3D3-56985A6D57BE}" name="Bonne pratique à adopter" dataDxfId="3"/>
     <tableColumn id="5" xr3:uid="{D4090782-153B-B745-8747-522ACAF6A5EB}" name="Action recommandée" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{7DD18BAA-95ED-C642-8863-3D6C66C78033}" name="Référence" dataDxfId="0"/>
-    <tableColumn id="7" xr3:uid="{0B8FBB93-CD44-6B49-B0E8-50644C7F0099}" name="OK ?" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{7DD18BAA-95ED-C642-8863-3D6C66C78033}" name="Référence" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{0B8FBB93-CD44-6B49-B0E8-50644C7F0099}" name="OK ?" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -931,7 +943,7 @@
   <dimension ref="A1:Z1014"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E39" sqref="E39"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1728,8 +1740,22 @@
     </row>
     <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B38" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
     <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
W3C HTML CSS OK & 100% SEO
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fred/Desktop/OpenClassRoom/P4 Vrac/ProjetP4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9A75649-79B8-0F49-82BF-6D185CCE5391}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF489ABA-D9B9-A74E-8283-CF1284DE65BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="1160" windowWidth="46580" windowHeight="24620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="137">
   <si>
     <t>Problème identifié</t>
   </si>
@@ -439,6 +439,9 @@
   </si>
   <si>
     <t>Erreur a regarder</t>
+  </si>
+  <si>
+    <t>jsquery sur page d'index emmerdais la performance et ne servait a rien</t>
   </si>
 </sst>
 </file>
@@ -942,8 +945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z1014"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1756,7 +1759,11 @@
         <v>135</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C39" s="1" t="s">
+        <v>136</v>
+      </c>
+    </row>
     <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
W3C HTML CSS OK & 100% SEO TABLO OK
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fred/Desktop/OpenClassRoom/P4 Vrac/ProjetP4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF489ABA-D9B9-A74E-8283-CF1284DE65BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{378B287D-4FBD-0345-80DC-E062D5B518E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1920" yWindow="1160" windowWidth="46580" windowHeight="24620" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="141">
   <si>
     <t>Problème identifié</t>
   </si>
@@ -93,9 +93,6 @@
     <t>CAT</t>
   </si>
   <si>
-    <t>Accesibilité</t>
-  </si>
-  <si>
     <t>Lien caché BlackHat</t>
   </si>
   <si>
@@ -393,9 +390,6 @@
     <t>Mettre le Label dans le input puis le fermer</t>
   </si>
   <si>
-    <t>Les personnes seront enfin quel est le input demandé grace a une meilleure définition</t>
-  </si>
-  <si>
     <t>Rajout du focus</t>
   </si>
   <si>
@@ -432,23 +426,41 @@
     <t>Correction sur le W3CC en CSS</t>
   </si>
   <si>
-    <t>plein d'erreur bootstrap</t>
-  </si>
-  <si>
-    <t>Correction sur le W3CC en html</t>
-  </si>
-  <si>
-    <t>Erreur a regarder</t>
-  </si>
-  <si>
-    <t>jsquery sur page d'index emmerdais la performance et ne servait a rien</t>
+    <t>Erreurs corrigées</t>
+  </si>
+  <si>
+    <t>Correction sur le W3CC en HTML</t>
+  </si>
+  <si>
+    <t>Plein d'erreurs du  bootstrap.css  et du style.css</t>
+  </si>
+  <si>
+    <t>Erreurs à regarder des erreurs de fermeture de div</t>
+  </si>
+  <si>
+    <t>En plus de vulnérabilité il ne servait a rien dans la page index.html</t>
+  </si>
+  <si>
+    <t>Enlevé les performances sont nettement meilleures</t>
+  </si>
+  <si>
+    <t>DIVERS</t>
+  </si>
+  <si>
+    <t>ACCESSIBLITE</t>
+  </si>
+  <si>
+    <t>DEMANDE DIRECTION</t>
+  </si>
+  <si>
+    <t>Les personnes seront enfin quel est le input  grace a une meilleure définition</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -507,6 +519,41 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="4"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -561,7 +608,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -587,12 +634,54 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="9">
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -618,30 +707,6 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
     </dxf>
     <dxf>
       <font>
@@ -730,16 +795,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E796EE32-1DFE-CD45-A2AF-F728FFC58B5F}" name="Tableau1" displayName="Tableau1" ref="A1:G34" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
-  <autoFilter ref="A1:G34" xr:uid="{E796EE32-1DFE-CD45-A2AF-F728FFC58B5F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{E796EE32-1DFE-CD45-A2AF-F728FFC58B5F}" name="Tableau1" displayName="Tableau1" ref="A1:G38" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
+  <autoFilter ref="A1:G38" xr:uid="{E796EE32-1DFE-CD45-A2AF-F728FFC58B5F}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{9BB85078-D1DA-EA4F-939E-EA2B94AC6A91}" name="CAT" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{701895DD-CBC8-C945-8BB8-1AF30E309D3E}" name="Problème identifié" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{8B278B00-9A53-D541-81DA-33000B0C5DCC}" name="Explication du problème" dataDxfId="4"/>
-    <tableColumn id="4" xr3:uid="{4C6455B9-1BC5-7D47-B3D3-56985A6D57BE}" name="Bonne pratique à adopter" dataDxfId="3"/>
-    <tableColumn id="5" xr3:uid="{D4090782-153B-B745-8747-522ACAF6A5EB}" name="Action recommandée" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{7DD18BAA-95ED-C642-8863-3D6C66C78033}" name="Référence" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{0B8FBB93-CD44-6B49-B0E8-50644C7F0099}" name="OK ?" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{9BB85078-D1DA-EA4F-939E-EA2B94AC6A91}" name="CAT" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{701895DD-CBC8-C945-8BB8-1AF30E309D3E}" name="Problème identifié" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{8B278B00-9A53-D541-81DA-33000B0C5DCC}" name="Explication du problème" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{4C6455B9-1BC5-7D47-B3D3-56985A6D57BE}" name="Bonne pratique à adopter" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{D4090782-153B-B745-8747-522ACAF6A5EB}" name="Action recommandée" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{7DD18BAA-95ED-C642-8863-3D6C66C78033}" name="Référence" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{0B8FBB93-CD44-6B49-B0E8-50644C7F0099}" name="OK ?" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -943,19 +1008,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z1014"/>
+  <dimension ref="A1:Z1018"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="24.140625" style="17" customWidth="1"/>
     <col min="2" max="2" width="42.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="68.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="55.85546875" style="1" customWidth="1"/>
-    <col min="5" max="5" width="82.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="56.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="72.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="30.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="27" width="10.5703125" style="1" customWidth="1"/>
@@ -963,7 +1028,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="13" t="s">
         <v>19</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -1005,267 +1070,267 @@
       <c r="Z1" s="8"/>
     </row>
     <row r="2" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="E2" s="9" t="s">
-        <v>48</v>
-      </c>
       <c r="F2" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="E3" s="9" t="s">
-        <v>31</v>
-      </c>
       <c r="F3" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D4" s="5" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>32</v>
-      </c>
-      <c r="F4" s="10" t="s">
-        <v>33</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="E5" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="E5" s="9" t="s">
-        <v>27</v>
-      </c>
       <c r="F5" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>22</v>
-      </c>
       <c r="F6" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="E7" s="9" t="s">
-        <v>37</v>
-      </c>
       <c r="F7" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="E8" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="F8" s="10" t="s">
         <v>41</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>42</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>45</v>
-      </c>
       <c r="E9" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="D10" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>51</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C11" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="D11" s="5" t="s">
         <v>53</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>54</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="D12" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="E12" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="E12" s="9" t="s">
-        <v>58</v>
-      </c>
       <c r="F12" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C13" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D13" s="5"/>
       <c r="E13" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F13" s="10" t="s">
         <v>11</v>
@@ -1275,43 +1340,43 @@
       </c>
     </row>
     <row r="14" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C14" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="D14" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="E14" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="E14" s="9" t="s">
-        <v>64</v>
-      </c>
       <c r="F14" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>12</v>
       </c>
       <c r="C15" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15" s="6" t="s">
         <v>65</v>
       </c>
-      <c r="D15" s="6" t="s">
-        <v>66</v>
-      </c>
       <c r="E15" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F15" s="10" t="s">
         <v>11</v>
@@ -1321,66 +1386,66 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D16" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="E16" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="F16" s="10" t="s">
         <v>71</v>
-      </c>
-      <c r="F16" s="10" t="s">
-        <v>72</v>
       </c>
       <c r="G16" s="11" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B17" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="D17" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="D17" s="5" t="s">
-        <v>70</v>
-      </c>
       <c r="E17" s="9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F17" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B18" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C18" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="D18" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="D18" s="5" t="s">
-        <v>76</v>
-      </c>
       <c r="E18" s="5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F18" s="10" t="s">
         <v>11</v>
@@ -1390,20 +1455,20 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C19" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C19" s="5" t="s">
-        <v>78</v>
-      </c>
       <c r="D19" s="5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F19" s="10" t="s">
         <v>11</v>
@@ -1413,66 +1478,66 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C20" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="D20" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="E20" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="E20" s="9" t="s">
-        <v>81</v>
-      </c>
       <c r="F20" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B21" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="C21" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="C21" s="5" t="s">
+      <c r="D21" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="E21" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="E21" s="9" t="s">
-        <v>85</v>
-      </c>
       <c r="F21" s="10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="14" t="s">
         <v>5</v>
       </c>
       <c r="B22" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D22" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C22" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="D22" s="5" t="s">
+      <c r="E22" s="9" t="s">
         <v>87</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>88</v>
       </c>
       <c r="F22" s="10" t="s">
         <v>11</v>
@@ -1482,288 +1547,338 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="4"/>
+      <c r="A23" s="15"/>
       <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="9"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="11"/>
     </row>
     <row r="24" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="4" t="s">
-        <v>20</v>
+      <c r="A24" s="16" t="s">
+        <v>137</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>91</v>
+        <v>130</v>
       </c>
       <c r="C24" s="5" t="s">
-        <v>92</v>
+        <v>133</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>93</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>94</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="E24" s="9"/>
       <c r="F24" s="10" t="s">
-        <v>33</v>
+        <v>139</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="4" t="s">
-        <v>20</v>
+      <c r="A25" s="16" t="s">
+        <v>137</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>95</v>
+        <v>132</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>96</v>
+        <v>134</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>97</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>98</v>
-      </c>
+        <v>131</v>
+      </c>
+      <c r="E25" s="9"/>
       <c r="F25" s="10" t="s">
-        <v>72</v>
+        <v>139</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="4" t="s">
-        <v>20</v>
+      <c r="A26" s="16" t="s">
+        <v>137</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>99</v>
+        <v>67</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>100</v>
+        <v>135</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>103</v>
-      </c>
-      <c r="E26" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="F26" s="12" t="s">
-        <v>102</v>
+        <v>136</v>
+      </c>
+      <c r="E26" s="9"/>
+      <c r="F26" s="10" t="s">
+        <v>66</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="D27" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="E27" s="9" t="s">
-        <v>107</v>
-      </c>
-      <c r="F27" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>15</v>
-      </c>
+      <c r="A27" s="15"/>
+      <c r="B27" s="5"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="4"/>
     </row>
     <row r="28" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="4" t="s">
-        <v>20</v>
+      <c r="A28" s="18" t="s">
+        <v>138</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>109</v>
-      </c>
-      <c r="E28" s="5" t="s">
-        <v>110</v>
+        <v>92</v>
+      </c>
+      <c r="E28" s="9" t="s">
+        <v>93</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>67</v>
+        <v>32</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="4" t="s">
-        <v>20</v>
+      <c r="A29" s="18" t="s">
+        <v>138</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>18</v>
+        <v>94</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>112</v>
+        <v>95</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>113</v>
+        <v>96</v>
       </c>
       <c r="E29" s="9" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>33</v>
+        <v>71</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
-        <v>20</v>
+      <c r="A30" s="18" t="s">
+        <v>138</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>29</v>
+        <v>98</v>
       </c>
       <c r="C30" s="5" t="s">
-        <v>114</v>
+        <v>99</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="E30" s="9" t="s">
-        <v>116</v>
-      </c>
-      <c r="F30" s="10" t="s">
-        <v>33</v>
+        <v>102</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>101</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="4" t="s">
-        <v>20</v>
+      <c r="A31" s="18" t="s">
+        <v>138</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="C31" s="5" t="s">
-        <v>118</v>
+        <v>103</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>104</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="E31" s="9" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="F31" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G31" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="4" t="s">
-        <v>20</v>
+      <c r="A32" s="18" t="s">
+        <v>138</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
       <c r="C32" s="5" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>124</v>
+        <v>108</v>
+      </c>
+      <c r="E32" s="5" t="s">
+        <v>109</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="4" t="s">
-        <v>20</v>
+      <c r="A33" s="18" t="s">
+        <v>138</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>125</v>
+        <v>18</v>
       </c>
       <c r="C33" s="5" t="s">
-        <v>126</v>
+        <v>111</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="E33" s="5"/>
+        <v>112</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>93</v>
+      </c>
       <c r="F33" s="10" t="s">
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="G33" s="4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="4" t="s">
-        <v>20</v>
+      <c r="A34" s="18" t="s">
+        <v>138</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>131</v>
+        <v>28</v>
       </c>
       <c r="C34" s="5" t="s">
-        <v>128</v>
+        <v>113</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>129</v>
-      </c>
-      <c r="E34" s="5" t="s">
-        <v>130</v>
+        <v>114</v>
+      </c>
+      <c r="E34" s="9" t="s">
+        <v>115</v>
       </c>
       <c r="F34" s="10" t="s">
-        <v>72</v>
+        <v>32</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C39" s="1" t="s">
-        <v>136</v>
-      </c>
-    </row>
+    <row r="35" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>116</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E35" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="G35" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>120</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="E37" s="5"/>
+      <c r="F37" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="18" t="s">
+        <v>138</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>129</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="E38" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="F38" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="G38" s="4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2739,6 +2854,10 @@
     <row r="1012" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1013" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="1014" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1015" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1016" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1017" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="1018" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="C10" r:id="rId1" display="https://fredericguilet.github.io/P4Guillet_Frederic25072021/voiture.com" xr:uid="{F0E0A3CD-37FD-9E44-B979-49DC1760F2BE}"/>
@@ -2761,22 +2880,23 @@
     <hyperlink ref="F20" r:id="rId18" xr:uid="{9940974C-2DE6-C849-8FFF-E00D77703634}"/>
     <hyperlink ref="F21" r:id="rId19" xr:uid="{1ECF8826-8E64-8C4D-A5C5-F3A4B120FC8A}"/>
     <hyperlink ref="F22" r:id="rId20" xr:uid="{CCDE431B-14C3-8D46-8EAB-D188D8E8C8A5}"/>
-    <hyperlink ref="F24" r:id="rId21" xr:uid="{97697197-9AC2-DD4E-B736-F41F18C35D48}"/>
-    <hyperlink ref="F25" r:id="rId22" xr:uid="{1539DEE0-BB06-DB47-AF1C-6B209EF12EA0}"/>
-    <hyperlink ref="F26" r:id="rId23" xr:uid="{599ACF77-59D0-D14B-BE6E-6D952E5B07E0}"/>
-    <hyperlink ref="F27" r:id="rId24" xr:uid="{ED097B17-7FB9-9545-80E2-0E98276AA57C}"/>
-    <hyperlink ref="F28" r:id="rId25" xr:uid="{F00B7C1F-69A4-D940-BB2A-1A193C945363}"/>
-    <hyperlink ref="F29" r:id="rId26" xr:uid="{08D195A8-7329-AF49-8E35-335DF52BC222}"/>
-    <hyperlink ref="F30" r:id="rId27" xr:uid="{DA68F960-859B-194D-9CB5-2AB7FFB6A949}"/>
-    <hyperlink ref="F31" r:id="rId28" xr:uid="{76D83CA0-53C9-4B4F-A51A-49D6B94E80E3}"/>
-    <hyperlink ref="F32" r:id="rId29" xr:uid="{56FC4D89-7BAB-FC4C-8DDC-EC85DFE97FA8}"/>
-    <hyperlink ref="F33" r:id="rId30" xr:uid="{4DCD383E-1603-114E-83C8-FC52DEC40B13}"/>
-    <hyperlink ref="F34" r:id="rId31" xr:uid="{5BE6480B-CCB2-8044-87D5-FB762BC0C983}"/>
+    <hyperlink ref="F28" r:id="rId21" xr:uid="{97697197-9AC2-DD4E-B736-F41F18C35D48}"/>
+    <hyperlink ref="F29" r:id="rId22" xr:uid="{1539DEE0-BB06-DB47-AF1C-6B209EF12EA0}"/>
+    <hyperlink ref="F30" r:id="rId23" xr:uid="{599ACF77-59D0-D14B-BE6E-6D952E5B07E0}"/>
+    <hyperlink ref="F31" r:id="rId24" xr:uid="{ED097B17-7FB9-9545-80E2-0E98276AA57C}"/>
+    <hyperlink ref="F32" r:id="rId25" xr:uid="{F00B7C1F-69A4-D940-BB2A-1A193C945363}"/>
+    <hyperlink ref="F33" r:id="rId26" xr:uid="{08D195A8-7329-AF49-8E35-335DF52BC222}"/>
+    <hyperlink ref="F34" r:id="rId27" xr:uid="{DA68F960-859B-194D-9CB5-2AB7FFB6A949}"/>
+    <hyperlink ref="F35" r:id="rId28" xr:uid="{76D83CA0-53C9-4B4F-A51A-49D6B94E80E3}"/>
+    <hyperlink ref="F36" r:id="rId29" xr:uid="{56FC4D89-7BAB-FC4C-8DDC-EC85DFE97FA8}"/>
+    <hyperlink ref="F37" r:id="rId30" xr:uid="{4DCD383E-1603-114E-83C8-FC52DEC40B13}"/>
+    <hyperlink ref="F38" r:id="rId31" xr:uid="{5BE6480B-CCB2-8044-87D5-FB762BC0C983}"/>
+    <hyperlink ref="F26" r:id="rId32" xr:uid="{2E7B6F51-8122-DE41-9068-D809C62D087F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
   <tableParts count="1">
-    <tablePart r:id="rId32"/>
+    <tablePart r:id="rId33"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>